<commit_message>
disable filters in excel file
</commit_message>
<xml_diff>
--- a/import/220207 Påmeldte via sportsadmin - for import.xlsx
+++ b/import/220207 Påmeldte via sportsadmin - for import.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10209"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{821527A6-6E76-F54A-8158-EC0A662D0D2D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{75F466E5-690B-5140-8BC8-69A4D160F0A9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="35840" yWindow="-5900" windowWidth="51200" windowHeight="28300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -5386,11 +5386,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <sheetPr filterMode="1"/>
   <dimension ref="A1:AB391"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="114" zoomScaleNormal="121" workbookViewId="0">
-      <selection activeCell="H414" sqref="H414"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="P205" zoomScale="114" zoomScaleNormal="121" workbookViewId="0">
+      <selection activeCell="F246" sqref="F246"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -5504,7 +5503,7 @@
       </c>
       <c r="AB3" s="2"/>
     </row>
-    <row r="4" spans="1:28" hidden="1" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:28" x14ac:dyDescent="0.15">
       <c r="A4" s="4" t="s">
         <v>25</v>
       </c>
@@ -5567,7 +5566,7 @@
       </c>
       <c r="AB4" s="4"/>
     </row>
-    <row r="5" spans="1:28" hidden="1" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:28" x14ac:dyDescent="0.15">
       <c r="A5" s="4" t="s">
         <v>25</v>
       </c>
@@ -5630,7 +5629,7 @@
       </c>
       <c r="AB5" s="4"/>
     </row>
-    <row r="6" spans="1:28" hidden="1" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:28" x14ac:dyDescent="0.15">
       <c r="A6" s="4" t="s">
         <v>25</v>
       </c>
@@ -5695,7 +5694,7 @@
       </c>
       <c r="AB6" s="4"/>
     </row>
-    <row r="7" spans="1:28" hidden="1" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:28" x14ac:dyDescent="0.15">
       <c r="A7" s="4" t="s">
         <v>25</v>
       </c>
@@ -5762,7 +5761,7 @@
       </c>
       <c r="AB7" s="4"/>
     </row>
-    <row r="8" spans="1:28" hidden="1" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:28" x14ac:dyDescent="0.15">
       <c r="A8" s="4" t="s">
         <v>25</v>
       </c>
@@ -5827,7 +5826,7 @@
       </c>
       <c r="AB8" s="4"/>
     </row>
-    <row r="9" spans="1:28" hidden="1" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:28" x14ac:dyDescent="0.15">
       <c r="A9" s="4" t="s">
         <v>25</v>
       </c>
@@ -5892,7 +5891,7 @@
       </c>
       <c r="AB9" s="4"/>
     </row>
-    <row r="10" spans="1:28" hidden="1" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:28" x14ac:dyDescent="0.15">
       <c r="A10" s="4" t="s">
         <v>25</v>
       </c>
@@ -5957,7 +5956,7 @@
       </c>
       <c r="AB10" s="4"/>
     </row>
-    <row r="11" spans="1:28" hidden="1" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:28" x14ac:dyDescent="0.15">
       <c r="A11" s="4" t="s">
         <v>25</v>
       </c>
@@ -6022,7 +6021,7 @@
       </c>
       <c r="AB11" s="4"/>
     </row>
-    <row r="12" spans="1:28" ht="26" hidden="1" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:28" ht="26" x14ac:dyDescent="0.15">
       <c r="A12" s="4" t="s">
         <v>25</v>
       </c>
@@ -6087,7 +6086,7 @@
       </c>
       <c r="AB12" s="4"/>
     </row>
-    <row r="13" spans="1:28" hidden="1" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:28" x14ac:dyDescent="0.15">
       <c r="A13" s="4" t="s">
         <v>25</v>
       </c>
@@ -6152,7 +6151,7 @@
       </c>
       <c r="AB13" s="4"/>
     </row>
-    <row r="14" spans="1:28" hidden="1" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:28" x14ac:dyDescent="0.15">
       <c r="A14" s="4" t="s">
         <v>25</v>
       </c>
@@ -6215,7 +6214,7 @@
       </c>
       <c r="AB14" s="4"/>
     </row>
-    <row r="15" spans="1:28" ht="26" hidden="1" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:28" ht="26" x14ac:dyDescent="0.15">
       <c r="A15" s="4" t="s">
         <v>25</v>
       </c>
@@ -6278,7 +6277,7 @@
       </c>
       <c r="AB15" s="4"/>
     </row>
-    <row r="16" spans="1:28" hidden="1" x14ac:dyDescent="0.15">
+    <row r="16" spans="1:28" x14ac:dyDescent="0.15">
       <c r="A16" s="4" t="s">
         <v>25</v>
       </c>
@@ -6341,7 +6340,7 @@
       </c>
       <c r="AB16" s="4"/>
     </row>
-    <row r="17" spans="1:28" ht="26" hidden="1" x14ac:dyDescent="0.15">
+    <row r="17" spans="1:28" ht="26" x14ac:dyDescent="0.15">
       <c r="A17" s="4" t="s">
         <v>25</v>
       </c>
@@ -6404,7 +6403,7 @@
       </c>
       <c r="AB17" s="4"/>
     </row>
-    <row r="18" spans="1:28" hidden="1" x14ac:dyDescent="0.15">
+    <row r="18" spans="1:28" x14ac:dyDescent="0.15">
       <c r="A18" s="4" t="s">
         <v>25</v>
       </c>
@@ -6467,7 +6466,7 @@
       </c>
       <c r="AB18" s="4"/>
     </row>
-    <row r="19" spans="1:28" hidden="1" x14ac:dyDescent="0.15">
+    <row r="19" spans="1:28" x14ac:dyDescent="0.15">
       <c r="A19" s="4" t="s">
         <v>25</v>
       </c>
@@ -6530,7 +6529,7 @@
       </c>
       <c r="AB19" s="4"/>
     </row>
-    <row r="20" spans="1:28" hidden="1" x14ac:dyDescent="0.15">
+    <row r="20" spans="1:28" x14ac:dyDescent="0.15">
       <c r="A20" s="4" t="s">
         <v>25</v>
       </c>
@@ -6593,7 +6592,7 @@
       </c>
       <c r="AB20" s="4"/>
     </row>
-    <row r="21" spans="1:28" hidden="1" x14ac:dyDescent="0.15">
+    <row r="21" spans="1:28" x14ac:dyDescent="0.15">
       <c r="A21" s="4" t="s">
         <v>25</v>
       </c>
@@ -6656,7 +6655,7 @@
       </c>
       <c r="AB21" s="4"/>
     </row>
-    <row r="22" spans="1:28" hidden="1" x14ac:dyDescent="0.15">
+    <row r="22" spans="1:28" x14ac:dyDescent="0.15">
       <c r="A22" s="4" t="s">
         <v>25</v>
       </c>
@@ -6719,7 +6718,7 @@
       </c>
       <c r="AB22" s="4"/>
     </row>
-    <row r="23" spans="1:28" hidden="1" x14ac:dyDescent="0.15">
+    <row r="23" spans="1:28" x14ac:dyDescent="0.15">
       <c r="A23" s="4" t="s">
         <v>25</v>
       </c>
@@ -6782,7 +6781,7 @@
       </c>
       <c r="AB23" s="4"/>
     </row>
-    <row r="24" spans="1:28" hidden="1" x14ac:dyDescent="0.15">
+    <row r="24" spans="1:28" x14ac:dyDescent="0.15">
       <c r="A24" s="4" t="s">
         <v>25</v>
       </c>
@@ -6847,7 +6846,7 @@
       </c>
       <c r="AB24" s="4"/>
     </row>
-    <row r="25" spans="1:28" hidden="1" x14ac:dyDescent="0.15">
+    <row r="25" spans="1:28" x14ac:dyDescent="0.15">
       <c r="A25" s="4" t="s">
         <v>25</v>
       </c>
@@ -6910,7 +6909,7 @@
       </c>
       <c r="AB25" s="4"/>
     </row>
-    <row r="26" spans="1:28" ht="26" hidden="1" x14ac:dyDescent="0.15">
+    <row r="26" spans="1:28" ht="26" x14ac:dyDescent="0.15">
       <c r="A26" s="4" t="s">
         <v>25</v>
       </c>
@@ -6973,7 +6972,7 @@
       </c>
       <c r="AB26" s="4"/>
     </row>
-    <row r="27" spans="1:28" ht="26" hidden="1" x14ac:dyDescent="0.15">
+    <row r="27" spans="1:28" ht="26" x14ac:dyDescent="0.15">
       <c r="A27" s="4" t="s">
         <v>25</v>
       </c>
@@ -7036,7 +7035,7 @@
       </c>
       <c r="AB27" s="4"/>
     </row>
-    <row r="28" spans="1:28" ht="26" hidden="1" x14ac:dyDescent="0.15">
+    <row r="28" spans="1:28" ht="26" x14ac:dyDescent="0.15">
       <c r="A28" s="4" t="s">
         <v>25</v>
       </c>
@@ -7099,7 +7098,7 @@
       </c>
       <c r="AB28" s="4"/>
     </row>
-    <row r="29" spans="1:28" ht="26" hidden="1" x14ac:dyDescent="0.15">
+    <row r="29" spans="1:28" ht="26" x14ac:dyDescent="0.15">
       <c r="A29" s="4" t="s">
         <v>25</v>
       </c>
@@ -7162,7 +7161,7 @@
       </c>
       <c r="AB29" s="4"/>
     </row>
-    <row r="30" spans="1:28" hidden="1" x14ac:dyDescent="0.15">
+    <row r="30" spans="1:28" x14ac:dyDescent="0.15">
       <c r="A30" s="4" t="s">
         <v>198</v>
       </c>
@@ -7225,7 +7224,7 @@
       </c>
       <c r="AB30" s="4"/>
     </row>
-    <row r="31" spans="1:28" hidden="1" x14ac:dyDescent="0.15">
+    <row r="31" spans="1:28" x14ac:dyDescent="0.15">
       <c r="A31" s="4" t="s">
         <v>198</v>
       </c>
@@ -7288,7 +7287,7 @@
       </c>
       <c r="AB31" s="4"/>
     </row>
-    <row r="32" spans="1:28" ht="26" hidden="1" x14ac:dyDescent="0.15">
+    <row r="32" spans="1:28" ht="26" x14ac:dyDescent="0.15">
       <c r="A32" s="4" t="s">
         <v>198</v>
       </c>
@@ -7351,7 +7350,7 @@
       </c>
       <c r="AB32" s="4"/>
     </row>
-    <row r="33" spans="1:28" ht="26" hidden="1" x14ac:dyDescent="0.15">
+    <row r="33" spans="1:28" ht="26" x14ac:dyDescent="0.15">
       <c r="A33" s="4" t="s">
         <v>198</v>
       </c>
@@ -7414,7 +7413,7 @@
       </c>
       <c r="AB33" s="4"/>
     </row>
-    <row r="34" spans="1:28" ht="26" hidden="1" x14ac:dyDescent="0.15">
+    <row r="34" spans="1:28" ht="26" x14ac:dyDescent="0.15">
       <c r="A34" s="4" t="s">
         <v>198</v>
       </c>
@@ -7477,7 +7476,7 @@
       </c>
       <c r="AB34" s="4"/>
     </row>
-    <row r="35" spans="1:28" ht="26" hidden="1" x14ac:dyDescent="0.15">
+    <row r="35" spans="1:28" ht="26" x14ac:dyDescent="0.15">
       <c r="A35" s="4" t="s">
         <v>198</v>
       </c>
@@ -7540,7 +7539,7 @@
       </c>
       <c r="AB35" s="4"/>
     </row>
-    <row r="36" spans="1:28" ht="26" hidden="1" x14ac:dyDescent="0.15">
+    <row r="36" spans="1:28" ht="26" x14ac:dyDescent="0.15">
       <c r="A36" s="4" t="s">
         <v>198</v>
       </c>
@@ -7603,7 +7602,7 @@
       </c>
       <c r="AB36" s="4"/>
     </row>
-    <row r="37" spans="1:28" ht="26" hidden="1" x14ac:dyDescent="0.15">
+    <row r="37" spans="1:28" ht="26" x14ac:dyDescent="0.15">
       <c r="A37" s="4" t="s">
         <v>198</v>
       </c>
@@ -7666,7 +7665,7 @@
       </c>
       <c r="AB37" s="4"/>
     </row>
-    <row r="38" spans="1:28" hidden="1" x14ac:dyDescent="0.15">
+    <row r="38" spans="1:28" x14ac:dyDescent="0.15">
       <c r="A38" s="4" t="s">
         <v>198</v>
       </c>
@@ -7729,7 +7728,7 @@
       </c>
       <c r="AB38" s="4"/>
     </row>
-    <row r="39" spans="1:28" hidden="1" x14ac:dyDescent="0.15">
+    <row r="39" spans="1:28" x14ac:dyDescent="0.15">
       <c r="A39" s="4" t="s">
         <v>198</v>
       </c>
@@ -7792,7 +7791,7 @@
       </c>
       <c r="AB39" s="4"/>
     </row>
-    <row r="40" spans="1:28" hidden="1" x14ac:dyDescent="0.15">
+    <row r="40" spans="1:28" x14ac:dyDescent="0.15">
       <c r="A40" s="4" t="s">
         <v>198</v>
       </c>
@@ -7855,7 +7854,7 @@
       </c>
       <c r="AB40" s="4"/>
     </row>
-    <row r="41" spans="1:28" hidden="1" x14ac:dyDescent="0.15">
+    <row r="41" spans="1:28" x14ac:dyDescent="0.15">
       <c r="A41" s="4" t="s">
         <v>198</v>
       </c>
@@ -7920,7 +7919,7 @@
       </c>
       <c r="AB41" s="4"/>
     </row>
-    <row r="42" spans="1:28" hidden="1" x14ac:dyDescent="0.15">
+    <row r="42" spans="1:28" x14ac:dyDescent="0.15">
       <c r="A42" s="4" t="s">
         <v>198</v>
       </c>
@@ -7983,7 +7982,7 @@
       </c>
       <c r="AB42" s="4"/>
     </row>
-    <row r="43" spans="1:28" hidden="1" x14ac:dyDescent="0.15">
+    <row r="43" spans="1:28" x14ac:dyDescent="0.15">
       <c r="A43" s="4" t="s">
         <v>198</v>
       </c>
@@ -8048,7 +8047,7 @@
       </c>
       <c r="AB43" s="4"/>
     </row>
-    <row r="44" spans="1:28" ht="39" hidden="1" x14ac:dyDescent="0.15">
+    <row r="44" spans="1:28" ht="39" x14ac:dyDescent="0.15">
       <c r="A44" s="4" t="s">
         <v>198</v>
       </c>
@@ -8113,7 +8112,7 @@
       </c>
       <c r="AB44" s="4"/>
     </row>
-    <row r="45" spans="1:28" hidden="1" x14ac:dyDescent="0.15">
+    <row r="45" spans="1:28" x14ac:dyDescent="0.15">
       <c r="A45" s="4" t="s">
         <v>198</v>
       </c>
@@ -8176,7 +8175,7 @@
       </c>
       <c r="AB45" s="4"/>
     </row>
-    <row r="46" spans="1:28" ht="26" hidden="1" x14ac:dyDescent="0.15">
+    <row r="46" spans="1:28" ht="26" x14ac:dyDescent="0.15">
       <c r="A46" s="4" t="s">
         <v>288</v>
       </c>
@@ -8241,7 +8240,7 @@
       </c>
       <c r="AB46" s="4"/>
     </row>
-    <row r="47" spans="1:28" hidden="1" x14ac:dyDescent="0.15">
+    <row r="47" spans="1:28" x14ac:dyDescent="0.15">
       <c r="A47" s="4" t="s">
         <v>288</v>
       </c>
@@ -8306,7 +8305,7 @@
       </c>
       <c r="AB47" s="4"/>
     </row>
-    <row r="48" spans="1:28" hidden="1" x14ac:dyDescent="0.15">
+    <row r="48" spans="1:28" x14ac:dyDescent="0.15">
       <c r="A48" s="4" t="s">
         <v>288</v>
       </c>
@@ -8371,7 +8370,7 @@
       </c>
       <c r="AB48" s="4"/>
     </row>
-    <row r="49" spans="1:28" hidden="1" x14ac:dyDescent="0.15">
+    <row r="49" spans="1:28" x14ac:dyDescent="0.15">
       <c r="A49" s="4" t="s">
         <v>288</v>
       </c>
@@ -8436,7 +8435,7 @@
       </c>
       <c r="AB49" s="4"/>
     </row>
-    <row r="50" spans="1:28" ht="26" hidden="1" x14ac:dyDescent="0.15">
+    <row r="50" spans="1:28" ht="26" x14ac:dyDescent="0.15">
       <c r="A50" s="4" t="s">
         <v>288</v>
       </c>
@@ -8501,7 +8500,7 @@
       </c>
       <c r="AB50" s="4"/>
     </row>
-    <row r="51" spans="1:28" ht="26" hidden="1" x14ac:dyDescent="0.15">
+    <row r="51" spans="1:28" ht="26" x14ac:dyDescent="0.15">
       <c r="A51" s="4" t="s">
         <v>288</v>
       </c>
@@ -8564,7 +8563,7 @@
       </c>
       <c r="AB51" s="4"/>
     </row>
-    <row r="52" spans="1:28" hidden="1" x14ac:dyDescent="0.15">
+    <row r="52" spans="1:28" x14ac:dyDescent="0.15">
       <c r="A52" s="4" t="s">
         <v>288</v>
       </c>
@@ -8627,7 +8626,7 @@
       </c>
       <c r="AB52" s="4"/>
     </row>
-    <row r="53" spans="1:28" ht="26" hidden="1" x14ac:dyDescent="0.15">
+    <row r="53" spans="1:28" ht="26" x14ac:dyDescent="0.15">
       <c r="A53" s="4" t="s">
         <v>288</v>
       </c>
@@ -8690,7 +8689,7 @@
       </c>
       <c r="AB53" s="4"/>
     </row>
-    <row r="54" spans="1:28" hidden="1" x14ac:dyDescent="0.15">
+    <row r="54" spans="1:28" x14ac:dyDescent="0.15">
       <c r="A54" s="4" t="s">
         <v>288</v>
       </c>
@@ -8753,7 +8752,7 @@
       </c>
       <c r="AB54" s="4"/>
     </row>
-    <row r="55" spans="1:28" hidden="1" x14ac:dyDescent="0.15">
+    <row r="55" spans="1:28" x14ac:dyDescent="0.15">
       <c r="A55" s="4" t="s">
         <v>288</v>
       </c>
@@ -8816,7 +8815,7 @@
       </c>
       <c r="AB55" s="4"/>
     </row>
-    <row r="56" spans="1:28" ht="26" hidden="1" x14ac:dyDescent="0.15">
+    <row r="56" spans="1:28" ht="26" x14ac:dyDescent="0.15">
       <c r="A56" s="4" t="s">
         <v>288</v>
       </c>
@@ -8879,7 +8878,7 @@
       </c>
       <c r="AB56" s="4"/>
     </row>
-    <row r="57" spans="1:28" ht="26" hidden="1" x14ac:dyDescent="0.15">
+    <row r="57" spans="1:28" ht="26" x14ac:dyDescent="0.15">
       <c r="A57" s="4" t="s">
         <v>288</v>
       </c>
@@ -8942,7 +8941,7 @@
       </c>
       <c r="AB57" s="4"/>
     </row>
-    <row r="58" spans="1:28" ht="26" hidden="1" x14ac:dyDescent="0.15">
+    <row r="58" spans="1:28" ht="26" x14ac:dyDescent="0.15">
       <c r="A58" s="4" t="s">
         <v>288</v>
       </c>
@@ -9005,7 +9004,7 @@
       </c>
       <c r="AB58" s="4"/>
     </row>
-    <row r="59" spans="1:28" ht="26" hidden="1" x14ac:dyDescent="0.15">
+    <row r="59" spans="1:28" ht="26" x14ac:dyDescent="0.15">
       <c r="A59" s="4" t="s">
         <v>288</v>
       </c>
@@ -9070,7 +9069,7 @@
       </c>
       <c r="AB59" s="4"/>
     </row>
-    <row r="60" spans="1:28" ht="26" hidden="1" x14ac:dyDescent="0.15">
+    <row r="60" spans="1:28" ht="26" x14ac:dyDescent="0.15">
       <c r="A60" s="4" t="s">
         <v>288</v>
       </c>
@@ -9135,7 +9134,7 @@
       </c>
       <c r="AB60" s="4"/>
     </row>
-    <row r="61" spans="1:28" ht="26" hidden="1" x14ac:dyDescent="0.15">
+    <row r="61" spans="1:28" ht="26" x14ac:dyDescent="0.15">
       <c r="A61" s="4" t="s">
         <v>288</v>
       </c>
@@ -9198,7 +9197,7 @@
       </c>
       <c r="AB61" s="4"/>
     </row>
-    <row r="62" spans="1:28" ht="26" hidden="1" x14ac:dyDescent="0.15">
+    <row r="62" spans="1:28" ht="26" x14ac:dyDescent="0.15">
       <c r="A62" s="4" t="s">
         <v>288</v>
       </c>
@@ -9261,7 +9260,7 @@
       </c>
       <c r="AB62" s="4"/>
     </row>
-    <row r="63" spans="1:28" hidden="1" x14ac:dyDescent="0.15">
+    <row r="63" spans="1:28" x14ac:dyDescent="0.15">
       <c r="A63" s="4" t="s">
         <v>288</v>
       </c>
@@ -9324,7 +9323,7 @@
       </c>
       <c r="AB63" s="4"/>
     </row>
-    <row r="64" spans="1:28" hidden="1" x14ac:dyDescent="0.15">
+    <row r="64" spans="1:28" x14ac:dyDescent="0.15">
       <c r="A64" s="4" t="s">
         <v>288</v>
       </c>
@@ -9389,7 +9388,7 @@
       </c>
       <c r="AB64" s="4"/>
     </row>
-    <row r="65" spans="1:28" hidden="1" x14ac:dyDescent="0.15">
+    <row r="65" spans="1:28" x14ac:dyDescent="0.15">
       <c r="A65" s="4" t="s">
         <v>288</v>
       </c>
@@ -9454,7 +9453,7 @@
       </c>
       <c r="AB65" s="4"/>
     </row>
-    <row r="66" spans="1:28" hidden="1" x14ac:dyDescent="0.15">
+    <row r="66" spans="1:28" x14ac:dyDescent="0.15">
       <c r="A66" s="4" t="s">
         <v>288</v>
       </c>
@@ -9519,7 +9518,7 @@
       </c>
       <c r="AB66" s="4"/>
     </row>
-    <row r="67" spans="1:28" hidden="1" x14ac:dyDescent="0.15">
+    <row r="67" spans="1:28" x14ac:dyDescent="0.15">
       <c r="A67" s="4" t="s">
         <v>288</v>
       </c>
@@ -9582,7 +9581,7 @@
       </c>
       <c r="AB67" s="4"/>
     </row>
-    <row r="68" spans="1:28" hidden="1" x14ac:dyDescent="0.15">
+    <row r="68" spans="1:28" x14ac:dyDescent="0.15">
       <c r="A68" s="4" t="s">
         <v>288</v>
       </c>
@@ -9645,7 +9644,7 @@
       </c>
       <c r="AB68" s="4"/>
     </row>
-    <row r="69" spans="1:28" hidden="1" x14ac:dyDescent="0.15">
+    <row r="69" spans="1:28" x14ac:dyDescent="0.15">
       <c r="A69" s="4" t="s">
         <v>288</v>
       </c>
@@ -9708,7 +9707,7 @@
       </c>
       <c r="AB69" s="4"/>
     </row>
-    <row r="70" spans="1:28" hidden="1" x14ac:dyDescent="0.15">
+    <row r="70" spans="1:28" x14ac:dyDescent="0.15">
       <c r="A70" s="4" t="s">
         <v>288</v>
       </c>
@@ -9773,7 +9772,7 @@
       </c>
       <c r="AB70" s="4"/>
     </row>
-    <row r="71" spans="1:28" hidden="1" x14ac:dyDescent="0.15">
+    <row r="71" spans="1:28" x14ac:dyDescent="0.15">
       <c r="A71" s="4" t="s">
         <v>288</v>
       </c>
@@ -9836,7 +9835,7 @@
       </c>
       <c r="AB71" s="4"/>
     </row>
-    <row r="72" spans="1:28" hidden="1" x14ac:dyDescent="0.15">
+    <row r="72" spans="1:28" x14ac:dyDescent="0.15">
       <c r="A72" s="4" t="s">
         <v>422</v>
       </c>
@@ -9901,7 +9900,7 @@
       </c>
       <c r="AB72" s="4"/>
     </row>
-    <row r="73" spans="1:28" hidden="1" x14ac:dyDescent="0.15">
+    <row r="73" spans="1:28" x14ac:dyDescent="0.15">
       <c r="A73" s="4" t="s">
         <v>422</v>
       </c>
@@ -9964,7 +9963,7 @@
       </c>
       <c r="AB73" s="4"/>
     </row>
-    <row r="74" spans="1:28" hidden="1" x14ac:dyDescent="0.15">
+    <row r="74" spans="1:28" x14ac:dyDescent="0.15">
       <c r="A74" s="4" t="s">
         <v>422</v>
       </c>
@@ -10027,7 +10026,7 @@
       </c>
       <c r="AB74" s="4"/>
     </row>
-    <row r="75" spans="1:28" hidden="1" x14ac:dyDescent="0.15">
+    <row r="75" spans="1:28" x14ac:dyDescent="0.15">
       <c r="A75" s="4" t="s">
         <v>422</v>
       </c>
@@ -10090,7 +10089,7 @@
       </c>
       <c r="AB75" s="4"/>
     </row>
-    <row r="76" spans="1:28" ht="26" hidden="1" x14ac:dyDescent="0.15">
+    <row r="76" spans="1:28" ht="26" x14ac:dyDescent="0.15">
       <c r="A76" s="4" t="s">
         <v>422</v>
       </c>
@@ -10155,7 +10154,7 @@
       </c>
       <c r="AB76" s="4"/>
     </row>
-    <row r="77" spans="1:28" hidden="1" x14ac:dyDescent="0.15">
+    <row r="77" spans="1:28" x14ac:dyDescent="0.15">
       <c r="A77" s="4" t="s">
         <v>422</v>
       </c>
@@ -10218,7 +10217,7 @@
       </c>
       <c r="AB77" s="4"/>
     </row>
-    <row r="78" spans="1:28" hidden="1" x14ac:dyDescent="0.15">
+    <row r="78" spans="1:28" x14ac:dyDescent="0.15">
       <c r="A78" s="4" t="s">
         <v>422</v>
       </c>
@@ -10281,7 +10280,7 @@
       </c>
       <c r="AB78" s="4"/>
     </row>
-    <row r="79" spans="1:28" hidden="1" x14ac:dyDescent="0.15">
+    <row r="79" spans="1:28" x14ac:dyDescent="0.15">
       <c r="A79" s="4" t="s">
         <v>422</v>
       </c>
@@ -10344,7 +10343,7 @@
       </c>
       <c r="AB79" s="4"/>
     </row>
-    <row r="80" spans="1:28" hidden="1" x14ac:dyDescent="0.15">
+    <row r="80" spans="1:28" x14ac:dyDescent="0.15">
       <c r="A80" s="4" t="s">
         <v>465</v>
       </c>
@@ -10407,7 +10406,7 @@
       </c>
       <c r="AB80" s="4"/>
     </row>
-    <row r="81" spans="1:28" hidden="1" x14ac:dyDescent="0.15">
+    <row r="81" spans="1:28" x14ac:dyDescent="0.15">
       <c r="A81" s="4" t="s">
         <v>465</v>
       </c>
@@ -10470,7 +10469,7 @@
       </c>
       <c r="AB81" s="4"/>
     </row>
-    <row r="82" spans="1:28" hidden="1" x14ac:dyDescent="0.15">
+    <row r="82" spans="1:28" x14ac:dyDescent="0.15">
       <c r="A82" s="4" t="s">
         <v>465</v>
       </c>
@@ -10537,7 +10536,7 @@
       </c>
       <c r="AB82" s="4"/>
     </row>
-    <row r="83" spans="1:28" hidden="1" x14ac:dyDescent="0.15">
+    <row r="83" spans="1:28" x14ac:dyDescent="0.15">
       <c r="A83" s="4" t="s">
         <v>465</v>
       </c>
@@ -10604,7 +10603,7 @@
       </c>
       <c r="AB83" s="4"/>
     </row>
-    <row r="84" spans="1:28" hidden="1" x14ac:dyDescent="0.15">
+    <row r="84" spans="1:28" x14ac:dyDescent="0.15">
       <c r="A84" s="4" t="s">
         <v>487</v>
       </c>
@@ -10669,7 +10668,7 @@
       </c>
       <c r="AB84" s="4"/>
     </row>
-    <row r="85" spans="1:28" hidden="1" x14ac:dyDescent="0.15">
+    <row r="85" spans="1:28" x14ac:dyDescent="0.15">
       <c r="A85" s="4" t="s">
         <v>487</v>
       </c>
@@ -10734,7 +10733,7 @@
       </c>
       <c r="AB85" s="4"/>
     </row>
-    <row r="86" spans="1:28" hidden="1" x14ac:dyDescent="0.15">
+    <row r="86" spans="1:28" x14ac:dyDescent="0.15">
       <c r="A86" s="4" t="s">
         <v>487</v>
       </c>
@@ -10797,7 +10796,7 @@
       </c>
       <c r="AB86" s="4"/>
     </row>
-    <row r="87" spans="1:28" hidden="1" x14ac:dyDescent="0.15">
+    <row r="87" spans="1:28" x14ac:dyDescent="0.15">
       <c r="A87" s="4" t="s">
         <v>487</v>
       </c>
@@ -10860,7 +10859,7 @@
       </c>
       <c r="AB87" s="4"/>
     </row>
-    <row r="88" spans="1:28" hidden="1" x14ac:dyDescent="0.15">
+    <row r="88" spans="1:28" x14ac:dyDescent="0.15">
       <c r="A88" s="4" t="s">
         <v>487</v>
       </c>
@@ -10921,7 +10920,7 @@
       </c>
       <c r="AB88" s="4"/>
     </row>
-    <row r="89" spans="1:28" hidden="1" x14ac:dyDescent="0.15">
+    <row r="89" spans="1:28" x14ac:dyDescent="0.15">
       <c r="A89" s="4" t="s">
         <v>487</v>
       </c>
@@ -10984,7 +10983,7 @@
       </c>
       <c r="AB89" s="4"/>
     </row>
-    <row r="90" spans="1:28" ht="26" hidden="1" x14ac:dyDescent="0.15">
+    <row r="90" spans="1:28" ht="26" x14ac:dyDescent="0.15">
       <c r="A90" s="4" t="s">
         <v>513</v>
       </c>
@@ -11049,7 +11048,7 @@
       </c>
       <c r="AB90" s="4"/>
     </row>
-    <row r="91" spans="1:28" ht="26" hidden="1" x14ac:dyDescent="0.15">
+    <row r="91" spans="1:28" ht="26" x14ac:dyDescent="0.15">
       <c r="A91" s="6" t="s">
         <v>513</v>
       </c>
@@ -11114,7 +11113,7 @@
         <v>528</v>
       </c>
     </row>
-    <row r="92" spans="1:28" ht="26" hidden="1" x14ac:dyDescent="0.15">
+    <row r="92" spans="1:28" ht="26" x14ac:dyDescent="0.15">
       <c r="A92" s="4" t="s">
         <v>513</v>
       </c>
@@ -11177,7 +11176,7 @@
       </c>
       <c r="AB92" s="4"/>
     </row>
-    <row r="93" spans="1:28" hidden="1" x14ac:dyDescent="0.15">
+    <row r="93" spans="1:28" x14ac:dyDescent="0.15">
       <c r="A93" s="4" t="s">
         <v>513</v>
       </c>
@@ -11240,7 +11239,7 @@
       </c>
       <c r="AB93" s="4"/>
     </row>
-    <row r="94" spans="1:28" hidden="1" x14ac:dyDescent="0.15">
+    <row r="94" spans="1:28" x14ac:dyDescent="0.15">
       <c r="A94" s="4" t="s">
         <v>513</v>
       </c>
@@ -11303,7 +11302,7 @@
       </c>
       <c r="AB94" s="4"/>
     </row>
-    <row r="95" spans="1:28" hidden="1" x14ac:dyDescent="0.15">
+    <row r="95" spans="1:28" x14ac:dyDescent="0.15">
       <c r="A95" s="4" t="s">
         <v>513</v>
       </c>
@@ -11366,7 +11365,7 @@
       </c>
       <c r="AB95" s="4"/>
     </row>
-    <row r="96" spans="1:28" hidden="1" x14ac:dyDescent="0.15">
+    <row r="96" spans="1:28" x14ac:dyDescent="0.15">
       <c r="A96" s="4" t="s">
         <v>513</v>
       </c>
@@ -11429,7 +11428,7 @@
       </c>
       <c r="AB96" s="4"/>
     </row>
-    <row r="97" spans="1:28" ht="26" hidden="1" x14ac:dyDescent="0.15">
+    <row r="97" spans="1:28" ht="26" x14ac:dyDescent="0.15">
       <c r="A97" s="4" t="s">
         <v>513</v>
       </c>
@@ -11492,7 +11491,7 @@
       </c>
       <c r="AB97" s="4"/>
     </row>
-    <row r="98" spans="1:28" ht="26" hidden="1" x14ac:dyDescent="0.15">
+    <row r="98" spans="1:28" ht="26" x14ac:dyDescent="0.15">
       <c r="A98" s="4" t="s">
         <v>513</v>
       </c>
@@ -11555,7 +11554,7 @@
       </c>
       <c r="AB98" s="4"/>
     </row>
-    <row r="99" spans="1:28" hidden="1" x14ac:dyDescent="0.15">
+    <row r="99" spans="1:28" x14ac:dyDescent="0.15">
       <c r="A99" s="4" t="s">
         <v>513</v>
       </c>
@@ -11620,7 +11619,7 @@
       </c>
       <c r="AB99" s="4"/>
     </row>
-    <row r="100" spans="1:28" hidden="1" x14ac:dyDescent="0.15">
+    <row r="100" spans="1:28" x14ac:dyDescent="0.15">
       <c r="A100" s="4" t="s">
         <v>513</v>
       </c>
@@ -11685,7 +11684,7 @@
       </c>
       <c r="AB100" s="4"/>
     </row>
-    <row r="101" spans="1:28" hidden="1" x14ac:dyDescent="0.15">
+    <row r="101" spans="1:28" x14ac:dyDescent="0.15">
       <c r="A101" s="4" t="s">
         <v>513</v>
       </c>
@@ -11750,7 +11749,7 @@
       </c>
       <c r="AB101" s="4"/>
     </row>
-    <row r="102" spans="1:28" hidden="1" x14ac:dyDescent="0.15">
+    <row r="102" spans="1:28" x14ac:dyDescent="0.15">
       <c r="A102" s="4" t="s">
         <v>513</v>
       </c>
@@ -11815,7 +11814,7 @@
       </c>
       <c r="AB102" s="4"/>
     </row>
-    <row r="103" spans="1:28" hidden="1" x14ac:dyDescent="0.15">
+    <row r="103" spans="1:28" x14ac:dyDescent="0.15">
       <c r="A103" s="4" t="s">
         <v>513</v>
       </c>
@@ -11878,7 +11877,7 @@
       </c>
       <c r="AB103" s="4"/>
     </row>
-    <row r="104" spans="1:28" hidden="1" x14ac:dyDescent="0.15">
+    <row r="104" spans="1:28" x14ac:dyDescent="0.15">
       <c r="A104" s="4" t="s">
         <v>513</v>
       </c>
@@ -11941,7 +11940,7 @@
       </c>
       <c r="AB104" s="4"/>
     </row>
-    <row r="105" spans="1:28" hidden="1" x14ac:dyDescent="0.15">
+    <row r="105" spans="1:28" x14ac:dyDescent="0.15">
       <c r="A105" s="4" t="s">
         <v>513</v>
       </c>
@@ -12004,7 +12003,7 @@
       </c>
       <c r="AB105" s="4"/>
     </row>
-    <row r="106" spans="1:28" hidden="1" x14ac:dyDescent="0.15">
+    <row r="106" spans="1:28" x14ac:dyDescent="0.15">
       <c r="A106" s="4" t="s">
         <v>513</v>
       </c>
@@ -12065,7 +12064,7 @@
       </c>
       <c r="AB106" s="4"/>
     </row>
-    <row r="107" spans="1:28" hidden="1" x14ac:dyDescent="0.15">
+    <row r="107" spans="1:28" x14ac:dyDescent="0.15">
       <c r="A107" s="4" t="s">
         <v>513</v>
       </c>
@@ -12128,7 +12127,7 @@
       </c>
       <c r="AB107" s="4"/>
     </row>
-    <row r="108" spans="1:28" hidden="1" x14ac:dyDescent="0.15">
+    <row r="108" spans="1:28" x14ac:dyDescent="0.15">
       <c r="A108" s="4" t="s">
         <v>513</v>
       </c>
@@ -12191,7 +12190,7 @@
       </c>
       <c r="AB108" s="4"/>
     </row>
-    <row r="109" spans="1:28" ht="26" hidden="1" x14ac:dyDescent="0.15">
+    <row r="109" spans="1:28" ht="26" x14ac:dyDescent="0.15">
       <c r="A109" s="4" t="s">
         <v>513</v>
       </c>
@@ -12254,7 +12253,7 @@
       </c>
       <c r="AB109" s="4"/>
     </row>
-    <row r="110" spans="1:28" hidden="1" x14ac:dyDescent="0.15">
+    <row r="110" spans="1:28" x14ac:dyDescent="0.15">
       <c r="A110" s="4" t="s">
         <v>513</v>
       </c>
@@ -12317,7 +12316,7 @@
       </c>
       <c r="AB110" s="4"/>
     </row>
-    <row r="111" spans="1:28" ht="26" hidden="1" x14ac:dyDescent="0.15">
+    <row r="111" spans="1:28" ht="26" x14ac:dyDescent="0.15">
       <c r="A111" s="4" t="s">
         <v>513</v>
       </c>
@@ -12380,7 +12379,7 @@
       </c>
       <c r="AB111" s="4"/>
     </row>
-    <row r="112" spans="1:28" ht="26" hidden="1" x14ac:dyDescent="0.15">
+    <row r="112" spans="1:28" ht="26" x14ac:dyDescent="0.15">
       <c r="A112" s="4" t="s">
         <v>513</v>
       </c>
@@ -12443,7 +12442,7 @@
       </c>
       <c r="AB112" s="4"/>
     </row>
-    <row r="113" spans="1:28" hidden="1" x14ac:dyDescent="0.15">
+    <row r="113" spans="1:28" x14ac:dyDescent="0.15">
       <c r="A113" s="4" t="s">
         <v>513</v>
       </c>
@@ -12506,7 +12505,7 @@
       </c>
       <c r="AB113" s="4"/>
     </row>
-    <row r="114" spans="1:28" ht="26" hidden="1" x14ac:dyDescent="0.15">
+    <row r="114" spans="1:28" ht="26" x14ac:dyDescent="0.15">
       <c r="A114" s="6" t="s">
         <v>513</v>
       </c>
@@ -12571,7 +12570,7 @@
         <v>528</v>
       </c>
     </row>
-    <row r="115" spans="1:28" hidden="1" x14ac:dyDescent="0.15">
+    <row r="115" spans="1:28" x14ac:dyDescent="0.15">
       <c r="A115" s="4" t="s">
         <v>513</v>
       </c>
@@ -12636,7 +12635,7 @@
       </c>
       <c r="AB115" s="4"/>
     </row>
-    <row r="116" spans="1:28" hidden="1" x14ac:dyDescent="0.15">
+    <row r="116" spans="1:28" x14ac:dyDescent="0.15">
       <c r="A116" s="4" t="s">
         <v>513</v>
       </c>
@@ -12701,7 +12700,7 @@
       </c>
       <c r="AB116" s="4"/>
     </row>
-    <row r="117" spans="1:28" hidden="1" x14ac:dyDescent="0.15">
+    <row r="117" spans="1:28" x14ac:dyDescent="0.15">
       <c r="A117" s="4" t="s">
         <v>513</v>
       </c>
@@ -12766,7 +12765,7 @@
       </c>
       <c r="AB117" s="4"/>
     </row>
-    <row r="118" spans="1:28" hidden="1" x14ac:dyDescent="0.15">
+    <row r="118" spans="1:28" x14ac:dyDescent="0.15">
       <c r="A118" s="4" t="s">
         <v>513</v>
       </c>
@@ -12831,7 +12830,7 @@
       </c>
       <c r="AB118" s="4"/>
     </row>
-    <row r="119" spans="1:28" ht="26" hidden="1" x14ac:dyDescent="0.15">
+    <row r="119" spans="1:28" ht="26" x14ac:dyDescent="0.15">
       <c r="A119" s="4" t="s">
         <v>513</v>
       </c>
@@ -12894,7 +12893,7 @@
       </c>
       <c r="AB119" s="4"/>
     </row>
-    <row r="120" spans="1:28" ht="26" hidden="1" x14ac:dyDescent="0.15">
+    <row r="120" spans="1:28" ht="26" x14ac:dyDescent="0.15">
       <c r="A120" s="6" t="s">
         <v>513</v>
       </c>
@@ -12959,7 +12958,7 @@
         <v>528</v>
       </c>
     </row>
-    <row r="121" spans="1:28" hidden="1" x14ac:dyDescent="0.15">
+    <row r="121" spans="1:28" x14ac:dyDescent="0.15">
       <c r="A121" s="4" t="s">
         <v>513</v>
       </c>
@@ -13024,7 +13023,7 @@
       </c>
       <c r="AB121" s="4"/>
     </row>
-    <row r="122" spans="1:28" hidden="1" x14ac:dyDescent="0.15">
+    <row r="122" spans="1:28" x14ac:dyDescent="0.15">
       <c r="A122" s="4" t="s">
         <v>513</v>
       </c>
@@ -13089,7 +13088,7 @@
       </c>
       <c r="AB122" s="4"/>
     </row>
-    <row r="123" spans="1:28" hidden="1" x14ac:dyDescent="0.15">
+    <row r="123" spans="1:28" x14ac:dyDescent="0.15">
       <c r="A123" s="4" t="s">
         <v>513</v>
       </c>
@@ -13152,7 +13151,7 @@
       </c>
       <c r="AB123" s="4"/>
     </row>
-    <row r="124" spans="1:28" ht="26" hidden="1" x14ac:dyDescent="0.15">
+    <row r="124" spans="1:28" ht="26" x14ac:dyDescent="0.15">
       <c r="A124" s="4" t="s">
         <v>513</v>
       </c>
@@ -13215,7 +13214,7 @@
       </c>
       <c r="AB124" s="4"/>
     </row>
-    <row r="125" spans="1:28" ht="26" hidden="1" x14ac:dyDescent="0.15">
+    <row r="125" spans="1:28" ht="26" x14ac:dyDescent="0.15">
       <c r="A125" s="4" t="s">
         <v>513</v>
       </c>
@@ -13278,7 +13277,7 @@
       </c>
       <c r="AB125" s="4"/>
     </row>
-    <row r="126" spans="1:28" ht="26" hidden="1" x14ac:dyDescent="0.15">
+    <row r="126" spans="1:28" ht="26" x14ac:dyDescent="0.15">
       <c r="A126" s="4" t="s">
         <v>513</v>
       </c>
@@ -13341,7 +13340,7 @@
       </c>
       <c r="AB126" s="4"/>
     </row>
-    <row r="127" spans="1:28" ht="26" hidden="1" x14ac:dyDescent="0.15">
+    <row r="127" spans="1:28" ht="26" x14ac:dyDescent="0.15">
       <c r="A127" s="4" t="s">
         <v>513</v>
       </c>
@@ -13404,7 +13403,7 @@
       </c>
       <c r="AB127" s="4"/>
     </row>
-    <row r="128" spans="1:28" ht="26" hidden="1" x14ac:dyDescent="0.15">
+    <row r="128" spans="1:28" ht="26" x14ac:dyDescent="0.15">
       <c r="A128" s="4" t="s">
         <v>693</v>
       </c>
@@ -13467,7 +13466,7 @@
       </c>
       <c r="AB128" s="4"/>
     </row>
-    <row r="129" spans="1:28" ht="26" hidden="1" x14ac:dyDescent="0.15">
+    <row r="129" spans="1:28" ht="26" x14ac:dyDescent="0.15">
       <c r="A129" s="4" t="s">
         <v>693</v>
       </c>
@@ -13532,7 +13531,7 @@
       </c>
       <c r="AB129" s="4"/>
     </row>
-    <row r="130" spans="1:28" ht="26" hidden="1" x14ac:dyDescent="0.15">
+    <row r="130" spans="1:28" ht="26" x14ac:dyDescent="0.15">
       <c r="A130" s="4" t="s">
         <v>693</v>
       </c>
@@ -13595,7 +13594,7 @@
       </c>
       <c r="AB130" s="4"/>
     </row>
-    <row r="131" spans="1:28" hidden="1" x14ac:dyDescent="0.15">
+    <row r="131" spans="1:28" x14ac:dyDescent="0.15">
       <c r="A131" s="4" t="s">
         <v>693</v>
       </c>
@@ -13658,7 +13657,7 @@
       </c>
       <c r="AB131" s="4"/>
     </row>
-    <row r="132" spans="1:28" hidden="1" x14ac:dyDescent="0.15">
+    <row r="132" spans="1:28" x14ac:dyDescent="0.15">
       <c r="A132" s="4" t="s">
         <v>693</v>
       </c>
@@ -13721,7 +13720,7 @@
       </c>
       <c r="AB132" s="4"/>
     </row>
-    <row r="133" spans="1:28" ht="26" hidden="1" x14ac:dyDescent="0.15">
+    <row r="133" spans="1:28" ht="26" x14ac:dyDescent="0.15">
       <c r="A133" s="4" t="s">
         <v>693</v>
       </c>
@@ -13784,7 +13783,7 @@
       </c>
       <c r="AB133" s="4"/>
     </row>
-    <row r="134" spans="1:28" ht="26" hidden="1" x14ac:dyDescent="0.15">
+    <row r="134" spans="1:28" ht="26" x14ac:dyDescent="0.15">
       <c r="A134" s="4" t="s">
         <v>693</v>
       </c>
@@ -13847,7 +13846,7 @@
       </c>
       <c r="AB134" s="4"/>
     </row>
-    <row r="135" spans="1:28" ht="26" hidden="1" x14ac:dyDescent="0.15">
+    <row r="135" spans="1:28" ht="26" x14ac:dyDescent="0.15">
       <c r="A135" s="4" t="s">
         <v>693</v>
       </c>
@@ -13910,7 +13909,7 @@
       </c>
       <c r="AB135" s="4"/>
     </row>
-    <row r="136" spans="1:28" hidden="1" x14ac:dyDescent="0.15">
+    <row r="136" spans="1:28" x14ac:dyDescent="0.15">
       <c r="A136" s="4" t="s">
         <v>693</v>
       </c>
@@ -13973,7 +13972,7 @@
       </c>
       <c r="AB136" s="4"/>
     </row>
-    <row r="137" spans="1:28" ht="26" hidden="1" x14ac:dyDescent="0.15">
+    <row r="137" spans="1:28" ht="26" x14ac:dyDescent="0.15">
       <c r="A137" s="4" t="s">
         <v>693</v>
       </c>
@@ -14036,7 +14035,7 @@
       </c>
       <c r="AB137" s="4"/>
     </row>
-    <row r="138" spans="1:28" hidden="1" x14ac:dyDescent="0.15">
+    <row r="138" spans="1:28" x14ac:dyDescent="0.15">
       <c r="A138" s="4" t="s">
         <v>693</v>
       </c>
@@ -14099,7 +14098,7 @@
       </c>
       <c r="AB138" s="4"/>
     </row>
-    <row r="139" spans="1:28" hidden="1" x14ac:dyDescent="0.15">
+    <row r="139" spans="1:28" x14ac:dyDescent="0.15">
       <c r="A139" s="4" t="s">
         <v>693</v>
       </c>
@@ -14162,7 +14161,7 @@
       </c>
       <c r="AB139" s="4"/>
     </row>
-    <row r="140" spans="1:28" ht="26" hidden="1" x14ac:dyDescent="0.15">
+    <row r="140" spans="1:28" ht="26" x14ac:dyDescent="0.15">
       <c r="A140" s="4" t="s">
         <v>693</v>
       </c>
@@ -14225,7 +14224,7 @@
       </c>
       <c r="AB140" s="4"/>
     </row>
-    <row r="141" spans="1:28" ht="26" hidden="1" x14ac:dyDescent="0.15">
+    <row r="141" spans="1:28" ht="26" x14ac:dyDescent="0.15">
       <c r="A141" s="4" t="s">
         <v>693</v>
       </c>
@@ -14288,7 +14287,7 @@
       </c>
       <c r="AB141" s="4"/>
     </row>
-    <row r="142" spans="1:28" hidden="1" x14ac:dyDescent="0.15">
+    <row r="142" spans="1:28" x14ac:dyDescent="0.15">
       <c r="A142" s="4" t="s">
         <v>693</v>
       </c>
@@ -14351,7 +14350,7 @@
       </c>
       <c r="AB142" s="4"/>
     </row>
-    <row r="143" spans="1:28" hidden="1" x14ac:dyDescent="0.15">
+    <row r="143" spans="1:28" x14ac:dyDescent="0.15">
       <c r="A143" s="4" t="s">
         <v>693</v>
       </c>
@@ -14414,7 +14413,7 @@
       </c>
       <c r="AB143" s="4"/>
     </row>
-    <row r="144" spans="1:28" hidden="1" x14ac:dyDescent="0.15">
+    <row r="144" spans="1:28" x14ac:dyDescent="0.15">
       <c r="A144" s="4" t="s">
         <v>693</v>
       </c>
@@ -14477,7 +14476,7 @@
       </c>
       <c r="AB144" s="4"/>
     </row>
-    <row r="145" spans="1:28" ht="26" hidden="1" x14ac:dyDescent="0.15">
+    <row r="145" spans="1:28" ht="26" x14ac:dyDescent="0.15">
       <c r="A145" s="4" t="s">
         <v>693</v>
       </c>
@@ -14540,7 +14539,7 @@
       </c>
       <c r="AB145" s="4"/>
     </row>
-    <row r="146" spans="1:28" hidden="1" x14ac:dyDescent="0.15">
+    <row r="146" spans="1:28" x14ac:dyDescent="0.15">
       <c r="A146" s="4" t="s">
         <v>693</v>
       </c>
@@ -14603,7 +14602,7 @@
       </c>
       <c r="AB146" s="4"/>
     </row>
-    <row r="147" spans="1:28" ht="26" hidden="1" x14ac:dyDescent="0.15">
+    <row r="147" spans="1:28" ht="26" x14ac:dyDescent="0.15">
       <c r="A147" s="4" t="s">
         <v>693</v>
       </c>
@@ -14666,7 +14665,7 @@
       </c>
       <c r="AB147" s="4"/>
     </row>
-    <row r="148" spans="1:28" hidden="1" x14ac:dyDescent="0.15">
+    <row r="148" spans="1:28" x14ac:dyDescent="0.15">
       <c r="A148" s="4" t="s">
         <v>693</v>
       </c>
@@ -14729,7 +14728,7 @@
       </c>
       <c r="AB148" s="4"/>
     </row>
-    <row r="149" spans="1:28" ht="26" hidden="1" x14ac:dyDescent="0.15">
+    <row r="149" spans="1:28" ht="26" x14ac:dyDescent="0.15">
       <c r="A149" s="4" t="s">
         <v>693</v>
       </c>
@@ -14792,7 +14791,7 @@
       </c>
       <c r="AB149" s="4"/>
     </row>
-    <row r="150" spans="1:28" hidden="1" x14ac:dyDescent="0.15">
+    <row r="150" spans="1:28" x14ac:dyDescent="0.15">
       <c r="A150" s="4" t="s">
         <v>693</v>
       </c>
@@ -14855,7 +14854,7 @@
       </c>
       <c r="AB150" s="4"/>
     </row>
-    <row r="151" spans="1:28" hidden="1" x14ac:dyDescent="0.15">
+    <row r="151" spans="1:28" x14ac:dyDescent="0.15">
       <c r="A151" s="4" t="s">
         <v>693</v>
       </c>
@@ -14918,7 +14917,7 @@
       </c>
       <c r="AB151" s="4"/>
     </row>
-    <row r="152" spans="1:28" ht="26" hidden="1" x14ac:dyDescent="0.15">
+    <row r="152" spans="1:28" ht="26" x14ac:dyDescent="0.15">
       <c r="A152" s="4" t="s">
         <v>693</v>
       </c>
@@ -14981,7 +14980,7 @@
       </c>
       <c r="AB152" s="4"/>
     </row>
-    <row r="153" spans="1:28" ht="26" hidden="1" x14ac:dyDescent="0.15">
+    <row r="153" spans="1:28" ht="26" x14ac:dyDescent="0.15">
       <c r="A153" s="4" t="s">
         <v>693</v>
       </c>
@@ -15044,7 +15043,7 @@
       </c>
       <c r="AB153" s="4"/>
     </row>
-    <row r="154" spans="1:28" hidden="1" x14ac:dyDescent="0.15">
+    <row r="154" spans="1:28" x14ac:dyDescent="0.15">
       <c r="A154" s="4" t="s">
         <v>693</v>
       </c>
@@ -15107,7 +15106,7 @@
       </c>
       <c r="AB154" s="4"/>
     </row>
-    <row r="155" spans="1:28" hidden="1" x14ac:dyDescent="0.15">
+    <row r="155" spans="1:28" x14ac:dyDescent="0.15">
       <c r="A155" s="4" t="s">
         <v>693</v>
       </c>
@@ -15170,7 +15169,7 @@
       </c>
       <c r="AB155" s="4"/>
     </row>
-    <row r="156" spans="1:28" ht="26" hidden="1" x14ac:dyDescent="0.15">
+    <row r="156" spans="1:28" ht="26" x14ac:dyDescent="0.15">
       <c r="A156" s="4" t="s">
         <v>693</v>
       </c>
@@ -15233,7 +15232,7 @@
       </c>
       <c r="AB156" s="4"/>
     </row>
-    <row r="157" spans="1:28" hidden="1" x14ac:dyDescent="0.15">
+    <row r="157" spans="1:28" x14ac:dyDescent="0.15">
       <c r="A157" s="4" t="s">
         <v>693</v>
       </c>
@@ -15296,7 +15295,7 @@
       </c>
       <c r="AB157" s="4"/>
     </row>
-    <row r="158" spans="1:28" hidden="1" x14ac:dyDescent="0.15">
+    <row r="158" spans="1:28" x14ac:dyDescent="0.15">
       <c r="A158" s="4" t="s">
         <v>693</v>
       </c>
@@ -15359,7 +15358,7 @@
       </c>
       <c r="AB158" s="4"/>
     </row>
-    <row r="159" spans="1:28" hidden="1" x14ac:dyDescent="0.15">
+    <row r="159" spans="1:28" x14ac:dyDescent="0.15">
       <c r="A159" s="4" t="s">
         <v>693</v>
       </c>
@@ -15422,7 +15421,7 @@
       </c>
       <c r="AB159" s="4"/>
     </row>
-    <row r="160" spans="1:28" hidden="1" x14ac:dyDescent="0.15">
+    <row r="160" spans="1:28" x14ac:dyDescent="0.15">
       <c r="A160" s="4" t="s">
         <v>693</v>
       </c>
@@ -15485,7 +15484,7 @@
       </c>
       <c r="AB160" s="4"/>
     </row>
-    <row r="161" spans="1:28" hidden="1" x14ac:dyDescent="0.15">
+    <row r="161" spans="1:28" x14ac:dyDescent="0.15">
       <c r="A161" s="4" t="s">
         <v>693</v>
       </c>
@@ -15548,7 +15547,7 @@
       </c>
       <c r="AB161" s="4"/>
     </row>
-    <row r="162" spans="1:28" hidden="1" x14ac:dyDescent="0.15">
+    <row r="162" spans="1:28" x14ac:dyDescent="0.15">
       <c r="A162" s="4" t="s">
         <v>851</v>
       </c>
@@ -15611,7 +15610,7 @@
       </c>
       <c r="AB162" s="4"/>
     </row>
-    <row r="163" spans="1:28" hidden="1" x14ac:dyDescent="0.15">
+    <row r="163" spans="1:28" x14ac:dyDescent="0.15">
       <c r="A163" s="4" t="s">
         <v>851</v>
       </c>
@@ -15674,7 +15673,7 @@
       </c>
       <c r="AB163" s="4"/>
     </row>
-    <row r="164" spans="1:28" ht="26" hidden="1" x14ac:dyDescent="0.15">
+    <row r="164" spans="1:28" ht="26" x14ac:dyDescent="0.15">
       <c r="A164" s="4" t="s">
         <v>851</v>
       </c>
@@ -15737,7 +15736,7 @@
       </c>
       <c r="AB164" s="4"/>
     </row>
-    <row r="165" spans="1:28" ht="26" hidden="1" x14ac:dyDescent="0.15">
+    <row r="165" spans="1:28" ht="26" x14ac:dyDescent="0.15">
       <c r="A165" s="4" t="s">
         <v>851</v>
       </c>
@@ -15800,7 +15799,7 @@
       </c>
       <c r="AB165" s="4"/>
     </row>
-    <row r="166" spans="1:28" hidden="1" x14ac:dyDescent="0.15">
+    <row r="166" spans="1:28" x14ac:dyDescent="0.15">
       <c r="A166" s="4" t="s">
         <v>851</v>
       </c>
@@ -15867,7 +15866,7 @@
       </c>
       <c r="AB166" s="4"/>
     </row>
-    <row r="167" spans="1:28" hidden="1" x14ac:dyDescent="0.15">
+    <row r="167" spans="1:28" x14ac:dyDescent="0.15">
       <c r="A167" s="4" t="s">
         <v>851</v>
       </c>
@@ -15934,7 +15933,7 @@
       </c>
       <c r="AB167" s="4"/>
     </row>
-    <row r="168" spans="1:28" hidden="1" x14ac:dyDescent="0.15">
+    <row r="168" spans="1:28" x14ac:dyDescent="0.15">
       <c r="A168" s="4" t="s">
         <v>851</v>
       </c>
@@ -15997,7 +15996,7 @@
       </c>
       <c r="AB168" s="4"/>
     </row>
-    <row r="169" spans="1:28" hidden="1" x14ac:dyDescent="0.15">
+    <row r="169" spans="1:28" x14ac:dyDescent="0.15">
       <c r="A169" s="4" t="s">
         <v>851</v>
       </c>
@@ -16062,7 +16061,7 @@
       </c>
       <c r="AB169" s="4"/>
     </row>
-    <row r="170" spans="1:28" ht="26" hidden="1" x14ac:dyDescent="0.15">
+    <row r="170" spans="1:28" ht="26" x14ac:dyDescent="0.15">
       <c r="A170" s="4" t="s">
         <v>851</v>
       </c>
@@ -16127,7 +16126,7 @@
       </c>
       <c r="AB170" s="4"/>
     </row>
-    <row r="171" spans="1:28" ht="26" hidden="1" x14ac:dyDescent="0.15">
+    <row r="171" spans="1:28" ht="26" x14ac:dyDescent="0.15">
       <c r="A171" s="4" t="s">
         <v>851</v>
       </c>
@@ -16190,7 +16189,7 @@
       </c>
       <c r="AB171" s="4"/>
     </row>
-    <row r="172" spans="1:28" ht="26" hidden="1" x14ac:dyDescent="0.15">
+    <row r="172" spans="1:28" ht="26" x14ac:dyDescent="0.15">
       <c r="A172" s="4" t="s">
         <v>851</v>
       </c>
@@ -16255,7 +16254,7 @@
       </c>
       <c r="AB172" s="4"/>
     </row>
-    <row r="173" spans="1:28" ht="26" hidden="1" x14ac:dyDescent="0.15">
+    <row r="173" spans="1:28" ht="26" x14ac:dyDescent="0.15">
       <c r="A173" s="4" t="s">
         <v>851</v>
       </c>
@@ -16320,7 +16319,7 @@
       </c>
       <c r="AB173" s="4"/>
     </row>
-    <row r="174" spans="1:28" hidden="1" x14ac:dyDescent="0.15">
+    <row r="174" spans="1:28" x14ac:dyDescent="0.15">
       <c r="A174" s="4" t="s">
         <v>851</v>
       </c>
@@ -16383,7 +16382,7 @@
       </c>
       <c r="AB174" s="4"/>
     </row>
-    <row r="175" spans="1:28" ht="26" hidden="1" x14ac:dyDescent="0.15">
+    <row r="175" spans="1:28" ht="26" x14ac:dyDescent="0.15">
       <c r="A175" s="4" t="s">
         <v>851</v>
       </c>
@@ -16446,7 +16445,7 @@
       </c>
       <c r="AB175" s="4"/>
     </row>
-    <row r="176" spans="1:28" hidden="1" x14ac:dyDescent="0.15">
+    <row r="176" spans="1:28" x14ac:dyDescent="0.15">
       <c r="A176" s="4" t="s">
         <v>912</v>
       </c>
@@ -16511,7 +16510,7 @@
       </c>
       <c r="AB176" s="4"/>
     </row>
-    <row r="177" spans="1:28" hidden="1" x14ac:dyDescent="0.15">
+    <row r="177" spans="1:28" x14ac:dyDescent="0.15">
       <c r="A177" s="4" t="s">
         <v>912</v>
       </c>
@@ -16574,7 +16573,7 @@
       </c>
       <c r="AB177" s="4"/>
     </row>
-    <row r="178" spans="1:28" ht="26" hidden="1" x14ac:dyDescent="0.15">
+    <row r="178" spans="1:28" ht="26" x14ac:dyDescent="0.15">
       <c r="A178" s="4" t="s">
         <v>912</v>
       </c>
@@ -16639,7 +16638,7 @@
       </c>
       <c r="AB178" s="4"/>
     </row>
-    <row r="179" spans="1:28" hidden="1" x14ac:dyDescent="0.15">
+    <row r="179" spans="1:28" x14ac:dyDescent="0.15">
       <c r="A179" s="4" t="s">
         <v>912</v>
       </c>
@@ -16702,7 +16701,7 @@
       </c>
       <c r="AB179" s="4"/>
     </row>
-    <row r="180" spans="1:28" hidden="1" x14ac:dyDescent="0.15">
+    <row r="180" spans="1:28" x14ac:dyDescent="0.15">
       <c r="A180" s="4" t="s">
         <v>912</v>
       </c>
@@ -16767,7 +16766,7 @@
       </c>
       <c r="AB180" s="4"/>
     </row>
-    <row r="181" spans="1:28" ht="26" hidden="1" x14ac:dyDescent="0.15">
+    <row r="181" spans="1:28" ht="26" x14ac:dyDescent="0.15">
       <c r="A181" s="4" t="s">
         <v>912</v>
       </c>
@@ -16832,7 +16831,7 @@
       </c>
       <c r="AB181" s="4"/>
     </row>
-    <row r="182" spans="1:28" hidden="1" x14ac:dyDescent="0.15">
+    <row r="182" spans="1:28" x14ac:dyDescent="0.15">
       <c r="A182" s="4" t="s">
         <v>912</v>
       </c>
@@ -16897,7 +16896,7 @@
       </c>
       <c r="AB182" s="4"/>
     </row>
-    <row r="183" spans="1:28" hidden="1" x14ac:dyDescent="0.15">
+    <row r="183" spans="1:28" x14ac:dyDescent="0.15">
       <c r="A183" s="4" t="s">
         <v>912</v>
       </c>
@@ -16960,7 +16959,7 @@
       </c>
       <c r="AB183" s="4"/>
     </row>
-    <row r="184" spans="1:28" ht="26" hidden="1" x14ac:dyDescent="0.15">
+    <row r="184" spans="1:28" ht="26" x14ac:dyDescent="0.15">
       <c r="A184" s="4" t="s">
         <v>912</v>
       </c>
@@ -17023,7 +17022,7 @@
       </c>
       <c r="AB184" s="4"/>
     </row>
-    <row r="185" spans="1:28" hidden="1" x14ac:dyDescent="0.15">
+    <row r="185" spans="1:28" x14ac:dyDescent="0.15">
       <c r="A185" s="4" t="s">
         <v>912</v>
       </c>
@@ -17086,7 +17085,7 @@
       </c>
       <c r="AB185" s="4"/>
     </row>
-    <row r="186" spans="1:28" hidden="1" x14ac:dyDescent="0.15">
+    <row r="186" spans="1:28" x14ac:dyDescent="0.15">
       <c r="A186" s="4" t="s">
         <v>912</v>
       </c>
@@ -17151,7 +17150,7 @@
       </c>
       <c r="AB186" s="4"/>
     </row>
-    <row r="187" spans="1:28" ht="26" hidden="1" x14ac:dyDescent="0.15">
+    <row r="187" spans="1:28" ht="26" x14ac:dyDescent="0.15">
       <c r="A187" s="4" t="s">
         <v>912</v>
       </c>
@@ -17214,7 +17213,7 @@
       </c>
       <c r="AB187" s="4"/>
     </row>
-    <row r="188" spans="1:28" hidden="1" x14ac:dyDescent="0.15">
+    <row r="188" spans="1:28" x14ac:dyDescent="0.15">
       <c r="A188" s="4" t="s">
         <v>912</v>
       </c>
@@ -17277,7 +17276,7 @@
       </c>
       <c r="AB188" s="4"/>
     </row>
-    <row r="189" spans="1:28" ht="26" hidden="1" x14ac:dyDescent="0.15">
+    <row r="189" spans="1:28" ht="26" x14ac:dyDescent="0.15">
       <c r="A189" s="4" t="s">
         <v>912</v>
       </c>
@@ -17340,7 +17339,7 @@
       </c>
       <c r="AB189" s="4"/>
     </row>
-    <row r="190" spans="1:28" hidden="1" x14ac:dyDescent="0.15">
+    <row r="190" spans="1:28" x14ac:dyDescent="0.15">
       <c r="A190" s="4" t="s">
         <v>912</v>
       </c>
@@ -17403,7 +17402,7 @@
       </c>
       <c r="AB190" s="4"/>
     </row>
-    <row r="191" spans="1:28" ht="26" hidden="1" x14ac:dyDescent="0.15">
+    <row r="191" spans="1:28" ht="26" x14ac:dyDescent="0.15">
       <c r="A191" s="4" t="s">
         <v>912</v>
       </c>
@@ -17468,7 +17467,7 @@
       </c>
       <c r="AB191" s="4"/>
     </row>
-    <row r="192" spans="1:28" ht="26" hidden="1" x14ac:dyDescent="0.15">
+    <row r="192" spans="1:28" ht="26" x14ac:dyDescent="0.15">
       <c r="A192" s="4" t="s">
         <v>912</v>
       </c>
@@ -17533,7 +17532,7 @@
       </c>
       <c r="AB192" s="4"/>
     </row>
-    <row r="193" spans="1:28" ht="26" hidden="1" x14ac:dyDescent="0.15">
+    <row r="193" spans="1:28" ht="26" x14ac:dyDescent="0.15">
       <c r="A193" s="4" t="s">
         <v>912</v>
       </c>
@@ -17598,7 +17597,7 @@
       </c>
       <c r="AB193" s="4"/>
     </row>
-    <row r="194" spans="1:28" ht="26" hidden="1" x14ac:dyDescent="0.15">
+    <row r="194" spans="1:28" ht="26" x14ac:dyDescent="0.15">
       <c r="A194" s="4" t="s">
         <v>912</v>
       </c>
@@ -17663,7 +17662,7 @@
       </c>
       <c r="AB194" s="4"/>
     </row>
-    <row r="195" spans="1:28" hidden="1" x14ac:dyDescent="0.15">
+    <row r="195" spans="1:28" x14ac:dyDescent="0.15">
       <c r="A195" s="4" t="s">
         <v>912</v>
       </c>
@@ -17726,7 +17725,7 @@
       </c>
       <c r="AB195" s="4"/>
     </row>
-    <row r="196" spans="1:28" hidden="1" x14ac:dyDescent="0.15">
+    <row r="196" spans="1:28" x14ac:dyDescent="0.15">
       <c r="A196" s="4" t="s">
         <v>1001</v>
       </c>
@@ -17793,7 +17792,7 @@
       </c>
       <c r="AB196" s="4"/>
     </row>
-    <row r="197" spans="1:28" ht="26" hidden="1" x14ac:dyDescent="0.15">
+    <row r="197" spans="1:28" ht="26" x14ac:dyDescent="0.15">
       <c r="A197" s="4" t="s">
         <v>1001</v>
       </c>
@@ -17858,7 +17857,7 @@
       </c>
       <c r="AB197" s="4"/>
     </row>
-    <row r="198" spans="1:28" hidden="1" x14ac:dyDescent="0.15">
+    <row r="198" spans="1:28" x14ac:dyDescent="0.15">
       <c r="A198" s="4" t="s">
         <v>1001</v>
       </c>
@@ -17923,7 +17922,7 @@
       </c>
       <c r="AB198" s="4"/>
     </row>
-    <row r="199" spans="1:28" hidden="1" x14ac:dyDescent="0.15">
+    <row r="199" spans="1:28" x14ac:dyDescent="0.15">
       <c r="A199" s="4" t="s">
         <v>1001</v>
       </c>
@@ -17986,7 +17985,7 @@
       </c>
       <c r="AB199" s="4"/>
     </row>
-    <row r="200" spans="1:28" hidden="1" x14ac:dyDescent="0.15">
+    <row r="200" spans="1:28" x14ac:dyDescent="0.15">
       <c r="A200" s="4" t="s">
         <v>1001</v>
       </c>
@@ -18053,7 +18052,7 @@
       </c>
       <c r="AB200" s="4"/>
     </row>
-    <row r="201" spans="1:28" hidden="1" x14ac:dyDescent="0.15">
+    <row r="201" spans="1:28" x14ac:dyDescent="0.15">
       <c r="A201" s="4" t="s">
         <v>1001</v>
       </c>
@@ -18118,7 +18117,7 @@
       </c>
       <c r="AB201" s="4"/>
     </row>
-    <row r="202" spans="1:28" hidden="1" x14ac:dyDescent="0.15">
+    <row r="202" spans="1:28" x14ac:dyDescent="0.15">
       <c r="A202" s="4" t="s">
         <v>1001</v>
       </c>
@@ -18181,7 +18180,7 @@
       </c>
       <c r="AB202" s="4"/>
     </row>
-    <row r="203" spans="1:28" hidden="1" x14ac:dyDescent="0.15">
+    <row r="203" spans="1:28" x14ac:dyDescent="0.15">
       <c r="A203" s="4" t="s">
         <v>1001</v>
       </c>
@@ -18246,7 +18245,7 @@
       </c>
       <c r="AB203" s="4"/>
     </row>
-    <row r="204" spans="1:28" ht="26" hidden="1" x14ac:dyDescent="0.15">
+    <row r="204" spans="1:28" ht="26" x14ac:dyDescent="0.15">
       <c r="A204" s="4" t="s">
         <v>1001</v>
       </c>
@@ -18311,7 +18310,7 @@
       </c>
       <c r="AB204" s="4"/>
     </row>
-    <row r="205" spans="1:28" ht="26" hidden="1" x14ac:dyDescent="0.15">
+    <row r="205" spans="1:28" ht="26" x14ac:dyDescent="0.15">
       <c r="A205" s="4" t="s">
         <v>1001</v>
       </c>
@@ -18374,7 +18373,7 @@
       </c>
       <c r="AB205" s="4"/>
     </row>
-    <row r="206" spans="1:28" hidden="1" x14ac:dyDescent="0.15">
+    <row r="206" spans="1:28" x14ac:dyDescent="0.15">
       <c r="A206" s="4" t="s">
         <v>1050</v>
       </c>
@@ -18439,7 +18438,7 @@
       </c>
       <c r="AB206" s="4"/>
     </row>
-    <row r="207" spans="1:28" hidden="1" x14ac:dyDescent="0.15">
+    <row r="207" spans="1:28" x14ac:dyDescent="0.15">
       <c r="A207" s="4" t="s">
         <v>1050</v>
       </c>
@@ -18504,7 +18503,7 @@
       </c>
       <c r="AB207" s="4"/>
     </row>
-    <row r="208" spans="1:28" hidden="1" x14ac:dyDescent="0.15">
+    <row r="208" spans="1:28" x14ac:dyDescent="0.15">
       <c r="A208" s="4" t="s">
         <v>1050</v>
       </c>
@@ -18569,7 +18568,7 @@
       </c>
       <c r="AB208" s="4"/>
     </row>
-    <row r="209" spans="1:28" hidden="1" x14ac:dyDescent="0.15">
+    <row r="209" spans="1:28" x14ac:dyDescent="0.15">
       <c r="A209" s="4" t="s">
         <v>1050</v>
       </c>
@@ -18632,7 +18631,7 @@
       </c>
       <c r="AB209" s="4"/>
     </row>
-    <row r="210" spans="1:28" ht="26" hidden="1" x14ac:dyDescent="0.15">
+    <row r="210" spans="1:28" ht="26" x14ac:dyDescent="0.15">
       <c r="A210" s="4" t="s">
         <v>1050</v>
       </c>
@@ -18695,7 +18694,7 @@
       </c>
       <c r="AB210" s="4"/>
     </row>
-    <row r="211" spans="1:28" hidden="1" x14ac:dyDescent="0.15">
+    <row r="211" spans="1:28" x14ac:dyDescent="0.15">
       <c r="A211" s="4" t="s">
         <v>1050</v>
       </c>
@@ -18760,7 +18759,7 @@
       </c>
       <c r="AB211" s="4"/>
     </row>
-    <row r="212" spans="1:28" hidden="1" x14ac:dyDescent="0.15">
+    <row r="212" spans="1:28" x14ac:dyDescent="0.15">
       <c r="A212" s="4" t="s">
         <v>1050</v>
       </c>
@@ -18825,7 +18824,7 @@
       </c>
       <c r="AB212" s="4"/>
     </row>
-    <row r="213" spans="1:28" ht="26" hidden="1" x14ac:dyDescent="0.15">
+    <row r="213" spans="1:28" ht="26" x14ac:dyDescent="0.15">
       <c r="A213" s="4" t="s">
         <v>1050</v>
       </c>
@@ -18890,7 +18889,7 @@
       </c>
       <c r="AB213" s="4"/>
     </row>
-    <row r="214" spans="1:28" hidden="1" x14ac:dyDescent="0.15">
+    <row r="214" spans="1:28" x14ac:dyDescent="0.15">
       <c r="A214" s="4" t="s">
         <v>1093</v>
       </c>
@@ -18953,7 +18952,7 @@
       </c>
       <c r="AB214" s="4"/>
     </row>
-    <row r="215" spans="1:28" hidden="1" x14ac:dyDescent="0.15">
+    <row r="215" spans="1:28" x14ac:dyDescent="0.15">
       <c r="A215" s="4" t="s">
         <v>1093</v>
       </c>
@@ -19016,7 +19015,7 @@
       </c>
       <c r="AB215" s="4"/>
     </row>
-    <row r="216" spans="1:28" hidden="1" x14ac:dyDescent="0.15">
+    <row r="216" spans="1:28" x14ac:dyDescent="0.15">
       <c r="A216" s="4" t="s">
         <v>1093</v>
       </c>
@@ -19079,7 +19078,7 @@
       </c>
       <c r="AB216" s="4"/>
     </row>
-    <row r="217" spans="1:28" ht="26" hidden="1" x14ac:dyDescent="0.15">
+    <row r="217" spans="1:28" ht="26" x14ac:dyDescent="0.15">
       <c r="A217" s="4" t="s">
         <v>1093</v>
       </c>
@@ -19142,7 +19141,7 @@
       </c>
       <c r="AB217" s="4"/>
     </row>
-    <row r="218" spans="1:28" hidden="1" x14ac:dyDescent="0.15">
+    <row r="218" spans="1:28" x14ac:dyDescent="0.15">
       <c r="A218" s="4" t="s">
         <v>1093</v>
       </c>
@@ -19205,7 +19204,7 @@
       </c>
       <c r="AB218" s="4"/>
     </row>
-    <row r="219" spans="1:28" hidden="1" x14ac:dyDescent="0.15">
+    <row r="219" spans="1:28" x14ac:dyDescent="0.15">
       <c r="A219" s="4" t="s">
         <v>1093</v>
       </c>
@@ -19268,7 +19267,7 @@
       </c>
       <c r="AB219" s="4"/>
     </row>
-    <row r="220" spans="1:28" ht="26" hidden="1" x14ac:dyDescent="0.15">
+    <row r="220" spans="1:28" ht="26" x14ac:dyDescent="0.15">
       <c r="A220" s="4" t="s">
         <v>1093</v>
       </c>
@@ -19331,7 +19330,7 @@
       </c>
       <c r="AB220" s="4"/>
     </row>
-    <row r="221" spans="1:28" ht="26" hidden="1" x14ac:dyDescent="0.15">
+    <row r="221" spans="1:28" ht="26" x14ac:dyDescent="0.15">
       <c r="A221" s="4" t="s">
         <v>1093</v>
       </c>
@@ -19394,7 +19393,7 @@
       </c>
       <c r="AB221" s="4"/>
     </row>
-    <row r="222" spans="1:28" ht="26" hidden="1" x14ac:dyDescent="0.15">
+    <row r="222" spans="1:28" ht="26" x14ac:dyDescent="0.15">
       <c r="A222" s="4" t="s">
         <v>1093</v>
       </c>
@@ -19457,7 +19456,7 @@
       </c>
       <c r="AB222" s="4"/>
     </row>
-    <row r="223" spans="1:28" ht="26" hidden="1" x14ac:dyDescent="0.15">
+    <row r="223" spans="1:28" ht="26" x14ac:dyDescent="0.15">
       <c r="A223" s="4" t="s">
         <v>1093</v>
       </c>
@@ -19520,7 +19519,7 @@
       </c>
       <c r="AB223" s="4"/>
     </row>
-    <row r="224" spans="1:28" hidden="1" x14ac:dyDescent="0.15">
+    <row r="224" spans="1:28" x14ac:dyDescent="0.15">
       <c r="A224" s="4" t="s">
         <v>1093</v>
       </c>
@@ -19583,7 +19582,7 @@
       </c>
       <c r="AB224" s="4"/>
     </row>
-    <row r="225" spans="1:28" hidden="1" x14ac:dyDescent="0.15">
+    <row r="225" spans="1:28" x14ac:dyDescent="0.15">
       <c r="A225" s="4" t="s">
         <v>1093</v>
       </c>
@@ -19646,7 +19645,7 @@
       </c>
       <c r="AB225" s="4"/>
     </row>
-    <row r="226" spans="1:28" ht="26" hidden="1" x14ac:dyDescent="0.15">
+    <row r="226" spans="1:28" ht="26" x14ac:dyDescent="0.15">
       <c r="A226" s="4" t="s">
         <v>1143</v>
       </c>
@@ -19709,7 +19708,7 @@
       </c>
       <c r="AB226" s="4"/>
     </row>
-    <row r="227" spans="1:28" ht="26" hidden="1" x14ac:dyDescent="0.15">
+    <row r="227" spans="1:28" ht="26" x14ac:dyDescent="0.15">
       <c r="A227" s="4" t="s">
         <v>1143</v>
       </c>
@@ -19772,7 +19771,7 @@
       </c>
       <c r="AB227" s="4"/>
     </row>
-    <row r="228" spans="1:28" ht="26" hidden="1" x14ac:dyDescent="0.15">
+    <row r="228" spans="1:28" ht="26" x14ac:dyDescent="0.15">
       <c r="A228" s="4" t="s">
         <v>1143</v>
       </c>
@@ -19835,7 +19834,7 @@
       </c>
       <c r="AB228" s="4"/>
     </row>
-    <row r="229" spans="1:28" hidden="1" x14ac:dyDescent="0.15">
+    <row r="229" spans="1:28" x14ac:dyDescent="0.15">
       <c r="A229" s="4" t="s">
         <v>1143</v>
       </c>
@@ -19898,7 +19897,7 @@
       </c>
       <c r="AB229" s="4"/>
     </row>
-    <row r="230" spans="1:28" hidden="1" x14ac:dyDescent="0.15">
+    <row r="230" spans="1:28" x14ac:dyDescent="0.15">
       <c r="A230" s="4" t="s">
         <v>1143</v>
       </c>
@@ -19961,7 +19960,7 @@
       </c>
       <c r="AB230" s="4"/>
     </row>
-    <row r="231" spans="1:28" hidden="1" x14ac:dyDescent="0.15">
+    <row r="231" spans="1:28" x14ac:dyDescent="0.15">
       <c r="A231" s="4" t="s">
         <v>1143</v>
       </c>
@@ -20024,7 +20023,7 @@
       </c>
       <c r="AB231" s="4"/>
     </row>
-    <row r="232" spans="1:28" hidden="1" x14ac:dyDescent="0.15">
+    <row r="232" spans="1:28" x14ac:dyDescent="0.15">
       <c r="A232" s="4" t="s">
         <v>1143</v>
       </c>
@@ -20087,7 +20086,7 @@
       </c>
       <c r="AB232" s="4"/>
     </row>
-    <row r="233" spans="1:28" hidden="1" x14ac:dyDescent="0.15">
+    <row r="233" spans="1:28" x14ac:dyDescent="0.15">
       <c r="A233" s="4" t="s">
         <v>1143</v>
       </c>
@@ -20150,7 +20149,7 @@
       </c>
       <c r="AB233" s="4"/>
     </row>
-    <row r="234" spans="1:28" ht="26" hidden="1" x14ac:dyDescent="0.15">
+    <row r="234" spans="1:28" ht="26" x14ac:dyDescent="0.15">
       <c r="A234" s="4" t="s">
         <v>1143</v>
       </c>
@@ -20213,7 +20212,7 @@
       </c>
       <c r="AB234" s="4"/>
     </row>
-    <row r="235" spans="1:28" hidden="1" x14ac:dyDescent="0.15">
+    <row r="235" spans="1:28" x14ac:dyDescent="0.15">
       <c r="A235" s="4" t="s">
         <v>1143</v>
       </c>
@@ -20276,7 +20275,7 @@
       </c>
       <c r="AB235" s="4"/>
     </row>
-    <row r="236" spans="1:28" hidden="1" x14ac:dyDescent="0.15">
+    <row r="236" spans="1:28" x14ac:dyDescent="0.15">
       <c r="A236" s="4" t="s">
         <v>1143</v>
       </c>
@@ -20339,7 +20338,7 @@
       </c>
       <c r="AB236" s="4"/>
     </row>
-    <row r="237" spans="1:28" hidden="1" x14ac:dyDescent="0.15">
+    <row r="237" spans="1:28" x14ac:dyDescent="0.15">
       <c r="A237" s="4" t="s">
         <v>1143</v>
       </c>
@@ -20402,7 +20401,7 @@
       </c>
       <c r="AB237" s="4"/>
     </row>
-    <row r="238" spans="1:28" hidden="1" x14ac:dyDescent="0.15">
+    <row r="238" spans="1:28" x14ac:dyDescent="0.15">
       <c r="A238" s="4" t="s">
         <v>1143</v>
       </c>
@@ -20465,7 +20464,7 @@
       </c>
       <c r="AB238" s="4"/>
     </row>
-    <row r="239" spans="1:28" hidden="1" x14ac:dyDescent="0.15">
+    <row r="239" spans="1:28" x14ac:dyDescent="0.15">
       <c r="A239" s="4" t="s">
         <v>1143</v>
       </c>
@@ -20528,7 +20527,7 @@
       </c>
       <c r="AB239" s="4"/>
     </row>
-    <row r="240" spans="1:28" hidden="1" x14ac:dyDescent="0.15">
+    <row r="240" spans="1:28" x14ac:dyDescent="0.15">
       <c r="A240" s="4" t="s">
         <v>1143</v>
       </c>
@@ -20591,7 +20590,7 @@
       </c>
       <c r="AB240" s="4"/>
     </row>
-    <row r="241" spans="1:28" hidden="1" x14ac:dyDescent="0.15">
+    <row r="241" spans="1:28" x14ac:dyDescent="0.15">
       <c r="A241" s="4" t="s">
         <v>1143</v>
       </c>
@@ -20654,7 +20653,7 @@
       </c>
       <c r="AB241" s="4"/>
     </row>
-    <row r="242" spans="1:28" hidden="1" x14ac:dyDescent="0.15">
+    <row r="242" spans="1:28" x14ac:dyDescent="0.15">
       <c r="A242" s="4" t="s">
         <v>487</v>
       </c>
@@ -20719,7 +20718,7 @@
         <v>1239</v>
       </c>
     </row>
-    <row r="243" spans="1:28" hidden="1" x14ac:dyDescent="0.15">
+    <row r="243" spans="1:28" x14ac:dyDescent="0.15">
       <c r="A243" s="4" t="s">
         <v>487</v>
       </c>
@@ -20784,7 +20783,7 @@
         <v>1239</v>
       </c>
     </row>
-    <row r="244" spans="1:28" hidden="1" x14ac:dyDescent="0.15">
+    <row r="244" spans="1:28" x14ac:dyDescent="0.15">
       <c r="A244" s="4" t="s">
         <v>487</v>
       </c>
@@ -20849,7 +20848,7 @@
         <v>1239</v>
       </c>
     </row>
-    <row r="245" spans="1:28" ht="26" hidden="1" x14ac:dyDescent="0.15">
+    <row r="245" spans="1:28" ht="26" x14ac:dyDescent="0.15">
       <c r="A245" s="4" t="s">
         <v>487</v>
       </c>
@@ -20914,7 +20913,7 @@
         <v>1239</v>
       </c>
     </row>
-    <row r="246" spans="1:28" hidden="1" x14ac:dyDescent="0.15">
+    <row r="246" spans="1:28" x14ac:dyDescent="0.15">
       <c r="A246" s="4" t="s">
         <v>1143</v>
       </c>
@@ -20981,7 +20980,7 @@
         <v>1239</v>
       </c>
     </row>
-    <row r="247" spans="1:28" ht="26" hidden="1" x14ac:dyDescent="0.15">
+    <row r="247" spans="1:28" ht="26" x14ac:dyDescent="0.15">
       <c r="A247" s="4" t="s">
         <v>1143</v>
       </c>
@@ -21048,7 +21047,7 @@
         <v>1239</v>
       </c>
     </row>
-    <row r="248" spans="1:28" hidden="1" x14ac:dyDescent="0.15">
+    <row r="248" spans="1:28" x14ac:dyDescent="0.15">
       <c r="A248" s="8" t="s">
         <v>487</v>
       </c>
@@ -21099,7 +21098,7 @@
         <v>1250</v>
       </c>
     </row>
-    <row r="249" spans="1:28" hidden="1" x14ac:dyDescent="0.15">
+    <row r="249" spans="1:28" x14ac:dyDescent="0.15">
       <c r="A249" s="8" t="s">
         <v>487</v>
       </c>
@@ -21150,7 +21149,7 @@
         <v>1250</v>
       </c>
     </row>
-    <row r="250" spans="1:28" hidden="1" x14ac:dyDescent="0.15">
+    <row r="250" spans="1:28" x14ac:dyDescent="0.15">
       <c r="A250" s="8" t="s">
         <v>487</v>
       </c>
@@ -21201,7 +21200,7 @@
         <v>1250</v>
       </c>
     </row>
-    <row r="251" spans="1:28" hidden="1" x14ac:dyDescent="0.15">
+    <row r="251" spans="1:28" x14ac:dyDescent="0.15">
       <c r="A251" s="8" t="s">
         <v>487</v>
       </c>
@@ -21252,7 +21251,7 @@
         <v>1250</v>
       </c>
     </row>
-    <row r="252" spans="1:28" hidden="1" x14ac:dyDescent="0.15">
+    <row r="252" spans="1:28" x14ac:dyDescent="0.15">
       <c r="A252" s="8" t="s">
         <v>1093</v>
       </c>
@@ -21303,7 +21302,7 @@
         <v>1250</v>
       </c>
     </row>
-    <row r="253" spans="1:28" hidden="1" x14ac:dyDescent="0.15">
+    <row r="253" spans="1:28" x14ac:dyDescent="0.15">
       <c r="A253" s="8" t="s">
         <v>1093</v>
       </c>
@@ -21354,7 +21353,7 @@
         <v>1250</v>
       </c>
     </row>
-    <row r="254" spans="1:28" hidden="1" x14ac:dyDescent="0.15">
+    <row r="254" spans="1:28" x14ac:dyDescent="0.15">
       <c r="A254" s="8" t="s">
         <v>487</v>
       </c>
@@ -21405,7 +21404,7 @@
         <v>1250</v>
       </c>
     </row>
-    <row r="255" spans="1:28" hidden="1" x14ac:dyDescent="0.15">
+    <row r="255" spans="1:28" x14ac:dyDescent="0.15">
       <c r="A255" s="8" t="s">
         <v>487</v>
       </c>
@@ -21456,7 +21455,7 @@
         <v>1250</v>
       </c>
     </row>
-    <row r="256" spans="1:28" hidden="1" x14ac:dyDescent="0.15">
+    <row r="256" spans="1:28" x14ac:dyDescent="0.15">
       <c r="A256" s="8" t="s">
         <v>487</v>
       </c>
@@ -21507,7 +21506,7 @@
         <v>1250</v>
       </c>
     </row>
-    <row r="257" spans="1:27" hidden="1" x14ac:dyDescent="0.15">
+    <row r="257" spans="1:27" x14ac:dyDescent="0.15">
       <c r="A257" s="8" t="s">
         <v>487</v>
       </c>
@@ -21558,7 +21557,7 @@
         <v>1250</v>
       </c>
     </row>
-    <row r="258" spans="1:27" hidden="1" x14ac:dyDescent="0.15">
+    <row r="258" spans="1:27" x14ac:dyDescent="0.15">
       <c r="A258" s="8" t="s">
         <v>487</v>
       </c>
@@ -21609,7 +21608,7 @@
         <v>1250</v>
       </c>
     </row>
-    <row r="259" spans="1:27" hidden="1" x14ac:dyDescent="0.15">
+    <row r="259" spans="1:27" x14ac:dyDescent="0.15">
       <c r="A259" s="8" t="s">
         <v>487</v>
       </c>
@@ -21660,7 +21659,7 @@
         <v>1250</v>
       </c>
     </row>
-    <row r="260" spans="1:27" hidden="1" x14ac:dyDescent="0.15">
+    <row r="260" spans="1:27" x14ac:dyDescent="0.15">
       <c r="A260" s="8" t="s">
         <v>487</v>
       </c>
@@ -21711,7 +21710,7 @@
         <v>1250</v>
       </c>
     </row>
-    <row r="261" spans="1:27" hidden="1" x14ac:dyDescent="0.15">
+    <row r="261" spans="1:27" x14ac:dyDescent="0.15">
       <c r="A261" s="8" t="s">
         <v>487</v>
       </c>
@@ -21762,7 +21761,7 @@
         <v>1250</v>
       </c>
     </row>
-    <row r="262" spans="1:27" hidden="1" x14ac:dyDescent="0.15">
+    <row r="262" spans="1:27" x14ac:dyDescent="0.15">
       <c r="A262" s="8" t="s">
         <v>487</v>
       </c>
@@ -21813,7 +21812,7 @@
         <v>1250</v>
       </c>
     </row>
-    <row r="263" spans="1:27" hidden="1" x14ac:dyDescent="0.15">
+    <row r="263" spans="1:27" x14ac:dyDescent="0.15">
       <c r="A263" s="8" t="s">
         <v>487</v>
       </c>
@@ -21864,7 +21863,7 @@
         <v>1250</v>
       </c>
     </row>
-    <row r="264" spans="1:27" hidden="1" x14ac:dyDescent="0.15">
+    <row r="264" spans="1:27" x14ac:dyDescent="0.15">
       <c r="A264" s="8" t="s">
         <v>1093</v>
       </c>
@@ -21915,7 +21914,7 @@
         <v>1250</v>
       </c>
     </row>
-    <row r="265" spans="1:27" hidden="1" x14ac:dyDescent="0.15">
+    <row r="265" spans="1:27" x14ac:dyDescent="0.15">
       <c r="A265" s="8" t="s">
         <v>1093</v>
       </c>
@@ -21966,7 +21965,7 @@
         <v>1250</v>
       </c>
     </row>
-    <row r="266" spans="1:27" hidden="1" x14ac:dyDescent="0.15">
+    <row r="266" spans="1:27" x14ac:dyDescent="0.15">
       <c r="A266" s="8" t="s">
         <v>1093</v>
       </c>
@@ -22017,7 +22016,7 @@
         <v>1250</v>
       </c>
     </row>
-    <row r="267" spans="1:27" hidden="1" x14ac:dyDescent="0.15">
+    <row r="267" spans="1:27" x14ac:dyDescent="0.15">
       <c r="A267" s="8" t="s">
         <v>1093</v>
       </c>
@@ -22068,7 +22067,7 @@
         <v>1250</v>
       </c>
     </row>
-    <row r="268" spans="1:27" hidden="1" x14ac:dyDescent="0.15">
+    <row r="268" spans="1:27" x14ac:dyDescent="0.15">
       <c r="A268" s="8" t="s">
         <v>1093</v>
       </c>
@@ -22119,7 +22118,7 @@
         <v>1250</v>
       </c>
     </row>
-    <row r="269" spans="1:27" hidden="1" x14ac:dyDescent="0.15">
+    <row r="269" spans="1:27" x14ac:dyDescent="0.15">
       <c r="A269" s="8" t="s">
         <v>1093</v>
       </c>
@@ -22170,7 +22169,7 @@
         <v>1250</v>
       </c>
     </row>
-    <row r="270" spans="1:27" hidden="1" x14ac:dyDescent="0.15">
+    <row r="270" spans="1:27" x14ac:dyDescent="0.15">
       <c r="A270" s="8" t="s">
         <v>1093</v>
       </c>
@@ -22221,7 +22220,7 @@
         <v>1250</v>
       </c>
     </row>
-    <row r="271" spans="1:27" hidden="1" x14ac:dyDescent="0.15">
+    <row r="271" spans="1:27" x14ac:dyDescent="0.15">
       <c r="A271" s="8" t="s">
         <v>1093</v>
       </c>
@@ -22272,7 +22271,7 @@
         <v>1250</v>
       </c>
     </row>
-    <row r="272" spans="1:27" hidden="1" x14ac:dyDescent="0.15">
+    <row r="272" spans="1:27" x14ac:dyDescent="0.15">
       <c r="A272" s="8" t="s">
         <v>1093</v>
       </c>
@@ -22323,7 +22322,7 @@
         <v>1250</v>
       </c>
     </row>
-    <row r="273" spans="1:27" hidden="1" x14ac:dyDescent="0.15">
+    <row r="273" spans="1:27" x14ac:dyDescent="0.15">
       <c r="A273" s="8" t="s">
         <v>1093</v>
       </c>
@@ -22374,7 +22373,7 @@
         <v>1250</v>
       </c>
     </row>
-    <row r="274" spans="1:27" hidden="1" x14ac:dyDescent="0.15">
+    <row r="274" spans="1:27" x14ac:dyDescent="0.15">
       <c r="A274" s="8" t="s">
         <v>1093</v>
       </c>
@@ -22425,7 +22424,7 @@
         <v>1250</v>
       </c>
     </row>
-    <row r="275" spans="1:27" hidden="1" x14ac:dyDescent="0.15">
+    <row r="275" spans="1:27" x14ac:dyDescent="0.15">
       <c r="A275" s="8" t="s">
         <v>1093</v>
       </c>
@@ -22476,7 +22475,7 @@
         <v>1250</v>
       </c>
     </row>
-    <row r="276" spans="1:27" hidden="1" x14ac:dyDescent="0.15">
+    <row r="276" spans="1:27" x14ac:dyDescent="0.15">
       <c r="A276" s="8" t="s">
         <v>1093</v>
       </c>
@@ -22527,7 +22526,7 @@
         <v>1250</v>
       </c>
     </row>
-    <row r="277" spans="1:27" hidden="1" x14ac:dyDescent="0.15">
+    <row r="277" spans="1:27" x14ac:dyDescent="0.15">
       <c r="A277" s="8" t="s">
         <v>1093</v>
       </c>
@@ -22578,7 +22577,7 @@
         <v>1250</v>
       </c>
     </row>
-    <row r="278" spans="1:27" hidden="1" x14ac:dyDescent="0.15">
+    <row r="278" spans="1:27" x14ac:dyDescent="0.15">
       <c r="A278" s="8" t="s">
         <v>1093</v>
       </c>
@@ -22629,7 +22628,7 @@
         <v>1250</v>
       </c>
     </row>
-    <row r="279" spans="1:27" hidden="1" x14ac:dyDescent="0.15">
+    <row r="279" spans="1:27" x14ac:dyDescent="0.15">
       <c r="A279" s="8" t="s">
         <v>1093</v>
       </c>
@@ -22680,7 +22679,7 @@
         <v>1250</v>
       </c>
     </row>
-    <row r="280" spans="1:27" hidden="1" x14ac:dyDescent="0.15">
+    <row r="280" spans="1:27" x14ac:dyDescent="0.15">
       <c r="A280" s="8" t="s">
         <v>1093</v>
       </c>
@@ -22731,7 +22730,7 @@
         <v>1250</v>
       </c>
     </row>
-    <row r="281" spans="1:27" hidden="1" x14ac:dyDescent="0.15">
+    <row r="281" spans="1:27" x14ac:dyDescent="0.15">
       <c r="A281" s="8" t="s">
         <v>1093</v>
       </c>
@@ -22782,7 +22781,7 @@
         <v>1250</v>
       </c>
     </row>
-    <row r="282" spans="1:27" hidden="1" x14ac:dyDescent="0.15">
+    <row r="282" spans="1:27" x14ac:dyDescent="0.15">
       <c r="A282" s="8" t="s">
         <v>288</v>
       </c>
@@ -22829,7 +22828,7 @@
       <c r="Z282" s="8"/>
       <c r="AA282" s="12"/>
     </row>
-    <row r="283" spans="1:27" hidden="1" x14ac:dyDescent="0.15">
+    <row r="283" spans="1:27" x14ac:dyDescent="0.15">
       <c r="A283" s="8" t="s">
         <v>288</v>
       </c>
@@ -22876,7 +22875,7 @@
       <c r="Z283" s="8"/>
       <c r="AA283" s="12"/>
     </row>
-    <row r="284" spans="1:27" hidden="1" x14ac:dyDescent="0.15">
+    <row r="284" spans="1:27" x14ac:dyDescent="0.15">
       <c r="A284" s="8" t="s">
         <v>288</v>
       </c>
@@ -22923,7 +22922,7 @@
       <c r="Z284" s="8"/>
       <c r="AA284" s="12"/>
     </row>
-    <row r="285" spans="1:27" hidden="1" x14ac:dyDescent="0.15">
+    <row r="285" spans="1:27" x14ac:dyDescent="0.15">
       <c r="A285" s="8" t="s">
         <v>288</v>
       </c>
@@ -22970,7 +22969,7 @@
       <c r="Z285" s="8"/>
       <c r="AA285" s="12"/>
     </row>
-    <row r="286" spans="1:27" hidden="1" x14ac:dyDescent="0.15">
+    <row r="286" spans="1:27" x14ac:dyDescent="0.15">
       <c r="A286" s="8" t="s">
         <v>288</v>
       </c>
@@ -23017,7 +23016,7 @@
       <c r="Z286" s="8"/>
       <c r="AA286" s="12"/>
     </row>
-    <row r="287" spans="1:27" hidden="1" x14ac:dyDescent="0.15">
+    <row r="287" spans="1:27" x14ac:dyDescent="0.15">
       <c r="A287" s="8" t="s">
         <v>288</v>
       </c>
@@ -23064,7 +23063,7 @@
       <c r="Z287" s="8"/>
       <c r="AA287" s="12"/>
     </row>
-    <row r="288" spans="1:27" hidden="1" x14ac:dyDescent="0.15">
+    <row r="288" spans="1:27" x14ac:dyDescent="0.15">
       <c r="A288" s="8" t="s">
         <v>288</v>
       </c>
@@ -23111,7 +23110,7 @@
       <c r="Z288" s="8"/>
       <c r="AA288" s="12"/>
     </row>
-    <row r="289" spans="1:27" hidden="1" x14ac:dyDescent="0.15">
+    <row r="289" spans="1:27" x14ac:dyDescent="0.15">
       <c r="A289" s="8" t="s">
         <v>288</v>
       </c>
@@ -23158,7 +23157,7 @@
       <c r="Z289" s="8"/>
       <c r="AA289" s="12"/>
     </row>
-    <row r="290" spans="1:27" hidden="1" x14ac:dyDescent="0.15">
+    <row r="290" spans="1:27" x14ac:dyDescent="0.15">
       <c r="A290" s="8" t="s">
         <v>288</v>
       </c>
@@ -23205,7 +23204,7 @@
       <c r="Z290" s="8"/>
       <c r="AA290" s="12"/>
     </row>
-    <row r="291" spans="1:27" hidden="1" x14ac:dyDescent="0.15">
+    <row r="291" spans="1:27" x14ac:dyDescent="0.15">
       <c r="A291" s="8" t="s">
         <v>288</v>
       </c>
@@ -23252,7 +23251,7 @@
       <c r="Z291" s="8"/>
       <c r="AA291" s="12"/>
     </row>
-    <row r="292" spans="1:27" hidden="1" x14ac:dyDescent="0.15">
+    <row r="292" spans="1:27" x14ac:dyDescent="0.15">
       <c r="A292" s="8" t="s">
         <v>288</v>
       </c>
@@ -23299,7 +23298,7 @@
       <c r="Z292" s="8"/>
       <c r="AA292" s="12"/>
     </row>
-    <row r="293" spans="1:27" hidden="1" x14ac:dyDescent="0.15">
+    <row r="293" spans="1:27" x14ac:dyDescent="0.15">
       <c r="A293" s="8" t="s">
         <v>288</v>
       </c>
@@ -23346,7 +23345,7 @@
       <c r="Z293" s="8"/>
       <c r="AA293" s="12"/>
     </row>
-    <row r="294" spans="1:27" hidden="1" x14ac:dyDescent="0.15">
+    <row r="294" spans="1:27" x14ac:dyDescent="0.15">
       <c r="A294" s="8" t="s">
         <v>288</v>
       </c>
@@ -23393,7 +23392,7 @@
       <c r="Z294" s="8"/>
       <c r="AA294" s="12"/>
     </row>
-    <row r="295" spans="1:27" hidden="1" x14ac:dyDescent="0.15">
+    <row r="295" spans="1:27" x14ac:dyDescent="0.15">
       <c r="A295" s="8" t="s">
         <v>288</v>
       </c>
@@ -23440,7 +23439,7 @@
       <c r="Z295" s="8"/>
       <c r="AA295" s="12"/>
     </row>
-    <row r="296" spans="1:27" hidden="1" x14ac:dyDescent="0.15">
+    <row r="296" spans="1:27" x14ac:dyDescent="0.15">
       <c r="A296" s="8" t="s">
         <v>288</v>
       </c>
@@ -23487,7 +23486,7 @@
       <c r="Z296" s="8"/>
       <c r="AA296" s="12"/>
     </row>
-    <row r="297" spans="1:27" hidden="1" x14ac:dyDescent="0.15">
+    <row r="297" spans="1:27" x14ac:dyDescent="0.15">
       <c r="A297" s="8" t="s">
         <v>288</v>
       </c>
@@ -23534,7 +23533,7 @@
       <c r="Z297" s="8"/>
       <c r="AA297" s="12"/>
     </row>
-    <row r="298" spans="1:27" hidden="1" x14ac:dyDescent="0.15">
+    <row r="298" spans="1:27" x14ac:dyDescent="0.15">
       <c r="A298" s="8" t="s">
         <v>288</v>
       </c>
@@ -23581,7 +23580,7 @@
       <c r="Z298" s="8"/>
       <c r="AA298" s="12"/>
     </row>
-    <row r="299" spans="1:27" hidden="1" x14ac:dyDescent="0.15">
+    <row r="299" spans="1:27" x14ac:dyDescent="0.15">
       <c r="A299" s="8" t="s">
         <v>288</v>
       </c>
@@ -23628,7 +23627,7 @@
       <c r="Z299" s="8"/>
       <c r="AA299" s="12"/>
     </row>
-    <row r="300" spans="1:27" hidden="1" x14ac:dyDescent="0.15">
+    <row r="300" spans="1:27" x14ac:dyDescent="0.15">
       <c r="A300" s="8" t="s">
         <v>912</v>
       </c>
@@ -23675,7 +23674,7 @@
       <c r="Z300" s="8"/>
       <c r="AA300" s="12"/>
     </row>
-    <row r="301" spans="1:27" hidden="1" x14ac:dyDescent="0.15">
+    <row r="301" spans="1:27" x14ac:dyDescent="0.15">
       <c r="A301" s="8" t="s">
         <v>912</v>
       </c>
@@ -23722,7 +23721,7 @@
       <c r="Z301" s="8"/>
       <c r="AA301" s="12"/>
     </row>
-    <row r="302" spans="1:27" hidden="1" x14ac:dyDescent="0.15">
+    <row r="302" spans="1:27" x14ac:dyDescent="0.15">
       <c r="A302" s="8" t="s">
         <v>912</v>
       </c>
@@ -23769,7 +23768,7 @@
       <c r="Z302" s="8"/>
       <c r="AA302" s="12"/>
     </row>
-    <row r="303" spans="1:27" hidden="1" x14ac:dyDescent="0.15">
+    <row r="303" spans="1:27" x14ac:dyDescent="0.15">
       <c r="A303" s="8" t="s">
         <v>912</v>
       </c>
@@ -23816,7 +23815,7 @@
       <c r="Z303" s="8"/>
       <c r="AA303" s="12"/>
     </row>
-    <row r="304" spans="1:27" hidden="1" x14ac:dyDescent="0.15">
+    <row r="304" spans="1:27" x14ac:dyDescent="0.15">
       <c r="A304" s="8" t="s">
         <v>912</v>
       </c>
@@ -23863,7 +23862,7 @@
       <c r="Z304" s="8"/>
       <c r="AA304" s="12"/>
     </row>
-    <row r="305" spans="1:27" hidden="1" x14ac:dyDescent="0.15">
+    <row r="305" spans="1:27" x14ac:dyDescent="0.15">
       <c r="A305" s="8" t="s">
         <v>912</v>
       </c>
@@ -23910,7 +23909,7 @@
       <c r="Z305" s="8"/>
       <c r="AA305" s="12"/>
     </row>
-    <row r="306" spans="1:27" hidden="1" x14ac:dyDescent="0.15">
+    <row r="306" spans="1:27" x14ac:dyDescent="0.15">
       <c r="A306" s="8" t="s">
         <v>422</v>
       </c>
@@ -23957,7 +23956,7 @@
       <c r="Z306" s="8"/>
       <c r="AA306" s="12"/>
     </row>
-    <row r="307" spans="1:27" hidden="1" x14ac:dyDescent="0.15">
+    <row r="307" spans="1:27" x14ac:dyDescent="0.15">
       <c r="A307" s="8" t="s">
         <v>422</v>
       </c>
@@ -24004,7 +24003,7 @@
       <c r="Z307" s="8"/>
       <c r="AA307" s="12"/>
     </row>
-    <row r="308" spans="1:27" hidden="1" x14ac:dyDescent="0.15">
+    <row r="308" spans="1:27" x14ac:dyDescent="0.15">
       <c r="A308" s="8" t="s">
         <v>422</v>
       </c>
@@ -24051,7 +24050,7 @@
       <c r="Z308" s="8"/>
       <c r="AA308" s="12"/>
     </row>
-    <row r="309" spans="1:27" hidden="1" x14ac:dyDescent="0.15">
+    <row r="309" spans="1:27" x14ac:dyDescent="0.15">
       <c r="A309" s="8" t="s">
         <v>422</v>
       </c>
@@ -24098,7 +24097,7 @@
       <c r="Z309" s="8"/>
       <c r="AA309" s="12"/>
     </row>
-    <row r="310" spans="1:27" hidden="1" x14ac:dyDescent="0.15">
+    <row r="310" spans="1:27" x14ac:dyDescent="0.15">
       <c r="A310" s="8" t="s">
         <v>422</v>
       </c>
@@ -24145,7 +24144,7 @@
       <c r="Z310" s="8"/>
       <c r="AA310" s="12"/>
     </row>
-    <row r="311" spans="1:27" hidden="1" x14ac:dyDescent="0.15">
+    <row r="311" spans="1:27" x14ac:dyDescent="0.15">
       <c r="A311" s="8" t="s">
         <v>422</v>
       </c>
@@ -24192,7 +24191,7 @@
       <c r="Z311" s="8"/>
       <c r="AA311" s="12"/>
     </row>
-    <row r="312" spans="1:27" hidden="1" x14ac:dyDescent="0.15">
+    <row r="312" spans="1:27" x14ac:dyDescent="0.15">
       <c r="A312" s="8" t="s">
         <v>422</v>
       </c>
@@ -24239,7 +24238,7 @@
       <c r="Z312" s="8"/>
       <c r="AA312" s="12"/>
     </row>
-    <row r="313" spans="1:27" hidden="1" x14ac:dyDescent="0.15">
+    <row r="313" spans="1:27" x14ac:dyDescent="0.15">
       <c r="A313" s="8" t="s">
         <v>422</v>
       </c>
@@ -24286,7 +24285,7 @@
       <c r="Z313" s="8"/>
       <c r="AA313" s="12"/>
     </row>
-    <row r="314" spans="1:27" hidden="1" x14ac:dyDescent="0.15">
+    <row r="314" spans="1:27" x14ac:dyDescent="0.15">
       <c r="A314" s="8" t="s">
         <v>465</v>
       </c>
@@ -24333,7 +24332,7 @@
       <c r="Z314" s="8"/>
       <c r="AA314" s="12"/>
     </row>
-    <row r="315" spans="1:27" hidden="1" x14ac:dyDescent="0.15">
+    <row r="315" spans="1:27" x14ac:dyDescent="0.15">
       <c r="A315" s="8" t="s">
         <v>465</v>
       </c>
@@ -24380,7 +24379,7 @@
       <c r="Z315" s="8"/>
       <c r="AA315" s="12"/>
     </row>
-    <row r="316" spans="1:27" hidden="1" x14ac:dyDescent="0.15">
+    <row r="316" spans="1:27" x14ac:dyDescent="0.15">
       <c r="A316" s="8" t="s">
         <v>1001</v>
       </c>
@@ -24427,7 +24426,7 @@
       <c r="Z316" s="8"/>
       <c r="AA316" s="12"/>
     </row>
-    <row r="317" spans="1:27" hidden="1" x14ac:dyDescent="0.15">
+    <row r="317" spans="1:27" x14ac:dyDescent="0.15">
       <c r="A317" s="8" t="s">
         <v>1001</v>
       </c>
@@ -24474,7 +24473,7 @@
       <c r="Z317" s="8"/>
       <c r="AA317" s="12"/>
     </row>
-    <row r="318" spans="1:27" hidden="1" x14ac:dyDescent="0.15">
+    <row r="318" spans="1:27" x14ac:dyDescent="0.15">
       <c r="A318" s="8" t="s">
         <v>1050</v>
       </c>
@@ -24521,7 +24520,7 @@
       <c r="Z318" s="8"/>
       <c r="AA318" s="12"/>
     </row>
-    <row r="319" spans="1:27" hidden="1" x14ac:dyDescent="0.15">
+    <row r="319" spans="1:27" x14ac:dyDescent="0.15">
       <c r="A319" s="8" t="s">
         <v>1050</v>
       </c>
@@ -24568,7 +24567,7 @@
       <c r="Z319" s="8"/>
       <c r="AA319" s="12"/>
     </row>
-    <row r="320" spans="1:27" hidden="1" x14ac:dyDescent="0.15">
+    <row r="320" spans="1:27" x14ac:dyDescent="0.15">
       <c r="A320" s="8" t="s">
         <v>1050</v>
       </c>
@@ -24615,7 +24614,7 @@
       <c r="Z320" s="8"/>
       <c r="AA320" s="12"/>
     </row>
-    <row r="321" spans="1:27" hidden="1" x14ac:dyDescent="0.15">
+    <row r="321" spans="1:27" x14ac:dyDescent="0.15">
       <c r="A321" s="8" t="s">
         <v>1050</v>
       </c>
@@ -24662,7 +24661,7 @@
       <c r="Z321" s="8"/>
       <c r="AA321" s="12"/>
     </row>
-    <row r="322" spans="1:27" hidden="1" x14ac:dyDescent="0.15">
+    <row r="322" spans="1:27" x14ac:dyDescent="0.15">
       <c r="A322" s="8" t="s">
         <v>1050</v>
       </c>
@@ -24709,7 +24708,7 @@
       <c r="Z322" s="8"/>
       <c r="AA322" s="12"/>
     </row>
-    <row r="323" spans="1:27" hidden="1" x14ac:dyDescent="0.15">
+    <row r="323" spans="1:27" x14ac:dyDescent="0.15">
       <c r="A323" s="8" t="s">
         <v>1050</v>
       </c>
@@ -26388,7 +26387,7 @@
         <v>1439</v>
       </c>
     </row>
-    <row r="356" spans="1:27" hidden="1" x14ac:dyDescent="0.15">
+    <row r="356" spans="1:27" x14ac:dyDescent="0.15">
       <c r="A356" s="26" t="s">
         <v>198</v>
       </c>
@@ -26439,7 +26438,7 @@
         <v>1514</v>
       </c>
     </row>
-    <row r="357" spans="1:27" hidden="1" x14ac:dyDescent="0.15">
+    <row r="357" spans="1:27" x14ac:dyDescent="0.15">
       <c r="A357" s="26" t="s">
         <v>198</v>
       </c>
@@ -26490,7 +26489,7 @@
         <v>1514</v>
       </c>
     </row>
-    <row r="358" spans="1:27" hidden="1" x14ac:dyDescent="0.15">
+    <row r="358" spans="1:27" x14ac:dyDescent="0.15">
       <c r="A358" s="8" t="s">
         <v>198</v>
       </c>
@@ -26541,7 +26540,7 @@
         <v>1514</v>
       </c>
     </row>
-    <row r="359" spans="1:27" hidden="1" x14ac:dyDescent="0.15">
+    <row r="359" spans="1:27" x14ac:dyDescent="0.15">
       <c r="A359" s="8" t="s">
         <v>198</v>
       </c>
@@ -26592,7 +26591,7 @@
         <v>1514</v>
       </c>
     </row>
-    <row r="360" spans="1:27" hidden="1" x14ac:dyDescent="0.15">
+    <row r="360" spans="1:27" x14ac:dyDescent="0.15">
       <c r="A360" s="26" t="s">
         <v>851</v>
       </c>
@@ -26643,7 +26642,7 @@
         <v>1514</v>
       </c>
     </row>
-    <row r="361" spans="1:27" hidden="1" x14ac:dyDescent="0.15">
+    <row r="361" spans="1:27" x14ac:dyDescent="0.15">
       <c r="A361" s="26" t="s">
         <v>851</v>
       </c>
@@ -26694,7 +26693,7 @@
         <v>1514</v>
       </c>
     </row>
-    <row r="362" spans="1:27" hidden="1" x14ac:dyDescent="0.15">
+    <row r="362" spans="1:27" x14ac:dyDescent="0.15">
       <c r="A362" s="8" t="s">
         <v>851</v>
       </c>
@@ -26745,7 +26744,7 @@
         <v>1514</v>
       </c>
     </row>
-    <row r="363" spans="1:27" hidden="1" x14ac:dyDescent="0.15">
+    <row r="363" spans="1:27" x14ac:dyDescent="0.15">
       <c r="A363" s="8" t="s">
         <v>851</v>
       </c>
@@ -26796,7 +26795,7 @@
         <v>1514</v>
       </c>
     </row>
-    <row r="364" spans="1:27" hidden="1" x14ac:dyDescent="0.15">
+    <row r="364" spans="1:27" x14ac:dyDescent="0.15">
       <c r="A364" s="26" t="s">
         <v>851</v>
       </c>
@@ -26847,7 +26846,7 @@
         <v>1514</v>
       </c>
     </row>
-    <row r="365" spans="1:27" hidden="1" x14ac:dyDescent="0.15">
+    <row r="365" spans="1:27" x14ac:dyDescent="0.15">
       <c r="A365" s="26" t="s">
         <v>851</v>
       </c>
@@ -26894,7 +26893,7 @@
       <c r="Z365" s="26"/>
       <c r="AA365" s="30"/>
     </row>
-    <row r="366" spans="1:27" hidden="1" x14ac:dyDescent="0.15">
+    <row r="366" spans="1:27" x14ac:dyDescent="0.15">
       <c r="A366" s="8" t="s">
         <v>851</v>
       </c>
@@ -26945,7 +26944,7 @@
         <v>1514</v>
       </c>
     </row>
-    <row r="367" spans="1:27" hidden="1" x14ac:dyDescent="0.15">
+    <row r="367" spans="1:27" x14ac:dyDescent="0.15">
       <c r="A367" s="8" t="s">
         <v>851</v>
       </c>
@@ -26996,7 +26995,7 @@
         <v>1514</v>
       </c>
     </row>
-    <row r="368" spans="1:27" hidden="1" x14ac:dyDescent="0.15">
+    <row r="368" spans="1:27" x14ac:dyDescent="0.15">
       <c r="A368" s="26" t="s">
         <v>851</v>
       </c>
@@ -27047,7 +27046,7 @@
         <v>1514</v>
       </c>
     </row>
-    <row r="369" spans="1:27" hidden="1" x14ac:dyDescent="0.15">
+    <row r="369" spans="1:27" x14ac:dyDescent="0.15">
       <c r="A369" s="26" t="s">
         <v>851</v>
       </c>
@@ -27094,7 +27093,7 @@
       <c r="Z369" s="26"/>
       <c r="AA369" s="30"/>
     </row>
-    <row r="370" spans="1:27" hidden="1" x14ac:dyDescent="0.15">
+    <row r="370" spans="1:27" x14ac:dyDescent="0.15">
       <c r="A370" s="8" t="s">
         <v>25</v>
       </c>
@@ -27145,7 +27144,7 @@
         <v>1544</v>
       </c>
     </row>
-    <row r="371" spans="1:27" hidden="1" x14ac:dyDescent="0.15">
+    <row r="371" spans="1:27" x14ac:dyDescent="0.15">
       <c r="A371" s="8" t="s">
         <v>25</v>
       </c>
@@ -27196,7 +27195,7 @@
         <v>1544</v>
       </c>
     </row>
-    <row r="372" spans="1:27" hidden="1" x14ac:dyDescent="0.15">
+    <row r="372" spans="1:27" x14ac:dyDescent="0.15">
       <c r="A372" s="8" t="s">
         <v>25</v>
       </c>
@@ -27247,7 +27246,7 @@
         <v>1544</v>
       </c>
     </row>
-    <row r="373" spans="1:27" hidden="1" x14ac:dyDescent="0.15">
+    <row r="373" spans="1:27" x14ac:dyDescent="0.15">
       <c r="A373" s="8" t="s">
         <v>25</v>
       </c>
@@ -27298,7 +27297,7 @@
         <v>1544</v>
       </c>
     </row>
-    <row r="374" spans="1:27" hidden="1" x14ac:dyDescent="0.15">
+    <row r="374" spans="1:27" x14ac:dyDescent="0.15">
       <c r="A374" s="8" t="s">
         <v>25</v>
       </c>
@@ -27349,7 +27348,7 @@
         <v>1544</v>
       </c>
     </row>
-    <row r="375" spans="1:27" hidden="1" x14ac:dyDescent="0.15">
+    <row r="375" spans="1:27" x14ac:dyDescent="0.15">
       <c r="A375" s="8" t="s">
         <v>25</v>
       </c>
@@ -27400,7 +27399,7 @@
         <v>1544</v>
       </c>
     </row>
-    <row r="376" spans="1:27" hidden="1" x14ac:dyDescent="0.15">
+    <row r="376" spans="1:27" x14ac:dyDescent="0.15">
       <c r="A376" s="8" t="s">
         <v>25</v>
       </c>
@@ -27451,7 +27450,7 @@
         <v>1544</v>
       </c>
     </row>
-    <row r="377" spans="1:27" hidden="1" x14ac:dyDescent="0.15">
+    <row r="377" spans="1:27" x14ac:dyDescent="0.15">
       <c r="A377" s="8" t="s">
         <v>25</v>
       </c>
@@ -27502,7 +27501,7 @@
         <v>1544</v>
       </c>
     </row>
-    <row r="378" spans="1:27" hidden="1" x14ac:dyDescent="0.15">
+    <row r="378" spans="1:27" x14ac:dyDescent="0.15">
       <c r="A378" s="8" t="s">
         <v>288</v>
       </c>
@@ -27553,7 +27552,7 @@
         <v>1544</v>
       </c>
     </row>
-    <row r="379" spans="1:27" hidden="1" x14ac:dyDescent="0.15">
+    <row r="379" spans="1:27" x14ac:dyDescent="0.15">
       <c r="A379" s="8" t="s">
         <v>288</v>
       </c>
@@ -27604,7 +27603,7 @@
         <v>1544</v>
       </c>
     </row>
-    <row r="380" spans="1:27" hidden="1" x14ac:dyDescent="0.15">
+    <row r="380" spans="1:27" x14ac:dyDescent="0.15">
       <c r="A380" s="8" t="s">
         <v>288</v>
       </c>
@@ -27655,7 +27654,7 @@
         <v>1544</v>
       </c>
     </row>
-    <row r="381" spans="1:27" hidden="1" x14ac:dyDescent="0.15">
+    <row r="381" spans="1:27" x14ac:dyDescent="0.15">
       <c r="A381" s="8" t="s">
         <v>288</v>
       </c>
@@ -27706,7 +27705,7 @@
         <v>1544</v>
       </c>
     </row>
-    <row r="382" spans="1:27" hidden="1" x14ac:dyDescent="0.15">
+    <row r="382" spans="1:27" x14ac:dyDescent="0.15">
       <c r="A382" s="8" t="s">
         <v>422</v>
       </c>
@@ -27757,7 +27756,7 @@
         <v>1544</v>
       </c>
     </row>
-    <row r="383" spans="1:27" hidden="1" x14ac:dyDescent="0.15">
+    <row r="383" spans="1:27" x14ac:dyDescent="0.15">
       <c r="A383" s="8" t="s">
         <v>422</v>
       </c>
@@ -27808,7 +27807,7 @@
         <v>1544</v>
       </c>
     </row>
-    <row r="384" spans="1:27" hidden="1" x14ac:dyDescent="0.15">
+    <row r="384" spans="1:27" x14ac:dyDescent="0.15">
       <c r="A384" s="8" t="s">
         <v>422</v>
       </c>
@@ -27859,7 +27858,7 @@
         <v>1544</v>
       </c>
     </row>
-    <row r="385" spans="1:27" hidden="1" x14ac:dyDescent="0.15">
+    <row r="385" spans="1:27" x14ac:dyDescent="0.15">
       <c r="A385" s="8" t="s">
         <v>422</v>
       </c>
@@ -27910,7 +27909,7 @@
         <v>1544</v>
       </c>
     </row>
-    <row r="386" spans="1:27" hidden="1" x14ac:dyDescent="0.15">
+    <row r="386" spans="1:27" x14ac:dyDescent="0.15">
       <c r="A386" s="8" t="s">
         <v>693</v>
       </c>
@@ -27961,7 +27960,7 @@
         <v>1544</v>
       </c>
     </row>
-    <row r="387" spans="1:27" hidden="1" x14ac:dyDescent="0.15">
+    <row r="387" spans="1:27" x14ac:dyDescent="0.15">
       <c r="A387" s="8" t="s">
         <v>693</v>
       </c>
@@ -28012,7 +28011,7 @@
         <v>1544</v>
       </c>
     </row>
-    <row r="388" spans="1:27" hidden="1" x14ac:dyDescent="0.15">
+    <row r="388" spans="1:27" x14ac:dyDescent="0.15">
       <c r="A388" s="8" t="s">
         <v>851</v>
       </c>
@@ -28063,7 +28062,7 @@
         <v>1544</v>
       </c>
     </row>
-    <row r="389" spans="1:27" hidden="1" x14ac:dyDescent="0.15">
+    <row r="389" spans="1:27" x14ac:dyDescent="0.15">
       <c r="A389" s="8" t="s">
         <v>851</v>
       </c>
@@ -28114,7 +28113,7 @@
         <v>1544</v>
       </c>
     </row>
-    <row r="390" spans="1:27" hidden="1" x14ac:dyDescent="0.15">
+    <row r="390" spans="1:27" x14ac:dyDescent="0.15">
       <c r="A390" s="8" t="s">
         <v>912</v>
       </c>
@@ -28165,7 +28164,7 @@
         <v>1544</v>
       </c>
     </row>
-    <row r="391" spans="1:27" hidden="1" x14ac:dyDescent="0.15">
+    <row r="391" spans="1:27" x14ac:dyDescent="0.15">
       <c r="A391" s="8" t="s">
         <v>912</v>
       </c>
@@ -28217,13 +28216,7 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A3:AB391" xr:uid="{00000000-0009-0000-0000-000000000000}">
-    <filterColumn colId="24">
-      <filters>
-        <filter val="Lasse Kollerud"/>
-      </filters>
-    </filterColumn>
-  </autoFilter>
+  <autoFilter ref="A3:AB391" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
   <phoneticPr fontId="0" type="noConversion"/>
   <hyperlinks>
     <hyperlink ref="AA324" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>

</xml_diff>